<commit_message>
Add grant categorization columns to special rules matrix
Added three new columns to track rules that grant other special rules:
- Grant Category: AURA (82), BUFF (65), MARK (25), DEBUFF (6), BOOST (7)
- Grants Rule: The name of the rule being granted
- Grant Target: SELF_UNIT, FRIENDLY_UNIT, ENEMY_UNIT, or SELF

This categorization helps determine how each granting rule should be
processed by the combat engine.
</commit_message>
<xml_diff>
--- a/docs/special_rules_review_matrix.xlsx
+++ b/docs/special_rules_review_matrix.xlsx
@@ -473,12 +473,12 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R506"/>
+  <dimension ref="A1:U506"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
       <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -595,6 +595,21 @@
           <t>Notes</t>
         </is>
       </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Grant Category</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Grants Rule</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Grant Target</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="40" customHeight="1">
       <c r="A2" s="4" t="inlineStr">
@@ -4811,6 +4826,21 @@
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Prime Brothers</t>
         </is>
       </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>Unstoppable</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="62" ht="40" customHeight="1">
       <c r="A62" s="4" t="inlineStr">
@@ -4879,6 +4909,21 @@
           <t>Type: Aura Special Rules. Armies: Ratmen Clans, Robot Legions, Wormhole Daemons of Change, Wormhole Daemons of Lust, Wormhole Daemons of Plague (+1 more)</t>
         </is>
       </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>Ambush</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="63" ht="40" customHeight="1">
       <c r="A63" s="4" t="inlineStr">
@@ -5143,6 +5188,21 @@
           <t>Type: Aura Special Rules. Armies: Alien Hives</t>
         </is>
       </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>Hit &amp; Run Fighter</t>
+        </is>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="67" ht="40" customHeight="1">
       <c r="A67" s="4" t="inlineStr">
@@ -5203,6 +5263,21 @@
           <t>Type: Aura Special Rules. Armies: Dwarf Guilds</t>
         </is>
       </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>Sturdy Boost</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="68" ht="40" customHeight="1">
       <c r="A68" s="4" t="inlineStr">
@@ -5331,6 +5406,21 @@
           <t>Type: Aura Special Rules. Armies: Elven Jesters</t>
         </is>
       </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>Counter-Attack</t>
+        </is>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="70" ht="40" customHeight="1">
       <c r="A70" s="4" t="inlineStr">
@@ -5389,6 +5479,21 @@
       <c r="R70" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: DAO Union, Rebel Guerrillas</t>
+        </is>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T70" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -5511,6 +5616,21 @@
           <t>Type: Aura Special Rules. Armies: Rebel Guerrillas</t>
         </is>
       </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T72" t="inlineStr">
+        <is>
+          <t>Furious</t>
+        </is>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="73" ht="40" customHeight="1">
       <c r="A73" s="4" t="inlineStr">
@@ -5571,6 +5691,21 @@
           <t>Type: Weapon. Armies: Saurian Starhost</t>
         </is>
       </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T73" t="inlineStr">
+        <is>
+          <t>Bane</t>
+        </is>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="74" ht="40" customHeight="1">
       <c r="A74" s="4" t="inlineStr">
@@ -5623,6 +5758,21 @@
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Blood Brothers, Blood Prime Brothers, Dark Brothers, Dark Prime Brothers (+7 more)</t>
         </is>
       </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr">
+        <is>
+          <t>Bane in melee</t>
+        </is>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="75" ht="40" customHeight="1">
       <c r="A75" s="4" t="inlineStr">
@@ -5687,6 +5837,21 @@
           <t>Type: Weapon. Armies: Human Defense Force</t>
         </is>
       </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T75" t="inlineStr">
+        <is>
+          <t>Bane in melee</t>
+        </is>
+      </c>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="76" ht="40" customHeight="1">
       <c r="A76" s="4" t="inlineStr">
@@ -5737,6 +5902,21 @@
       <c r="R76" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Blood Brothers, Blood Prime Brothers, Dark Brothers, Dark Prime Brothers (+8 more)</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T76" t="inlineStr">
+        <is>
+          <t>Bane when shooting</t>
+        </is>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -5935,6 +6115,16 @@
           <t>Type: Aura Special Rules. Armies: Dwarf Guilds</t>
         </is>
       </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="80" ht="40" customHeight="1">
       <c r="A80" s="4" t="inlineStr">
@@ -6063,6 +6253,21 @@
           <t>Type: Aura Special Rules. Armies: Soul-Snatcher Cults</t>
         </is>
       </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T81" t="inlineStr">
+        <is>
+          <t>Teleport</t>
+        </is>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="82" ht="40" customHeight="1">
       <c r="A82" s="4" t="inlineStr">
@@ -6259,6 +6464,21 @@
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Dark Brothers, Dark Prime Brothers, Prime Brothers, Watch Brothers (+1 more)</t>
         </is>
       </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T84" t="inlineStr">
+        <is>
+          <t>Shred</t>
+        </is>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="85" ht="40" customHeight="1">
       <c r="A85" s="4" t="inlineStr">
@@ -6317,6 +6537,21 @@
       <c r="R85" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Plague Disciples, Wormhole Daemons of Plague</t>
+        </is>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T85" t="inlineStr">
+        <is>
+          <t>Rapid Rush</t>
+        </is>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -6379,6 +6614,21 @@
           <t>Type: Aura Special Rules. Armies: High Elf Fleets</t>
         </is>
       </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T86" t="inlineStr">
+        <is>
+          <t>Highborn Boost</t>
+        </is>
+      </c>
+      <c r="U86" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="87" ht="40" customHeight="1">
       <c r="A87" s="4" t="inlineStr">
@@ -6437,6 +6687,21 @@
       <c r="R87" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Lust Disciples, Wormhole Daemons of Lust</t>
+        </is>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T87" t="inlineStr">
+        <is>
+          <t>Melee Evasion</t>
+        </is>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -6499,6 +6764,21 @@
           <t>Type: Aura Special Rules. Armies: Blood Brothers, Blood Prime Brothers</t>
         </is>
       </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T88" t="inlineStr">
+        <is>
+          <t>Evasive</t>
+        </is>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="89" ht="40" customHeight="1">
       <c r="A89" s="4" t="inlineStr">
@@ -6557,6 +6837,21 @@
       <c r="R89" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Blood Brothers, Blood Prime Brothers</t>
+        </is>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T89" t="inlineStr">
+        <is>
+          <t>Unstoppable</t>
+        </is>
+      </c>
+      <c r="U89" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -6955,6 +7250,21 @@
           <t>Type: Aura Special Rules. Armies: Human Inquisition, Plague Disciples, Wormhole Daemons of Change</t>
         </is>
       </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T95" t="inlineStr">
+        <is>
+          <t>Bounding</t>
+        </is>
+      </c>
+      <c r="U95" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="96" ht="40" customHeight="1">
       <c r="A96" s="4" t="inlineStr">
@@ -7359,6 +7669,21 @@
           <t>Type: Aura Special Rules. Armies: Change Disciples, Wormhole Daemons of Change</t>
         </is>
       </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T101" t="inlineStr">
+        <is>
+          <t>Bane</t>
+        </is>
+      </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="102" ht="40" customHeight="1">
       <c r="A102" s="4" t="inlineStr">
@@ -7555,6 +7880,21 @@
           <t>Type: Aura Special Rules. Armies: Blessed Sisters</t>
         </is>
       </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>DEBUFF</t>
+        </is>
+      </c>
+      <c r="T104" t="inlineStr">
+        <is>
+          <t>-3 to casting rolls</t>
+        </is>
+      </c>
+      <c r="U104" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="105" ht="40" customHeight="1">
       <c r="A105" s="4" t="inlineStr">
@@ -7615,6 +7955,21 @@
           <t>Type: Aura Special Rules. Armies: Blood Brothers, Blood Prime Brothers</t>
         </is>
       </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T105" t="inlineStr">
+        <is>
+          <t>Furious</t>
+        </is>
+      </c>
+      <c r="U105" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="106" ht="40" customHeight="1">
       <c r="A106" s="4" t="inlineStr">
@@ -7747,6 +8102,21 @@
           <t>Type: Aura Special Rules. Armies: Human Defense Force, Human Inquisition, Titan Lords</t>
         </is>
       </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T107" t="inlineStr">
+        <is>
+          <t>Relentless</t>
+        </is>
+      </c>
+      <c r="U107" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="108" ht="40" customHeight="1">
       <c r="A108" s="4" t="inlineStr">
@@ -7927,6 +8297,21 @@
           <t>Type: Unit. Armies: Blessed Sisters, Human Inquisition, Wormhole Daemons of Change</t>
         </is>
       </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>DEBUFF</t>
+        </is>
+      </c>
+      <c r="T110" t="inlineStr">
+        <is>
+          <t>-1 to casting rolls</t>
+        </is>
+      </c>
+      <c r="U110" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="111" ht="40" customHeight="1">
       <c r="A111" s="4" t="inlineStr">
@@ -7987,6 +8372,21 @@
           <t>Type: Aura Special Rules. Armies: Saurian Starhost</t>
         </is>
       </c>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T111" t="inlineStr">
+        <is>
+          <t>Primal Boost</t>
+        </is>
+      </c>
+      <c r="U111" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="112" ht="40" customHeight="1">
       <c r="A112" s="4" t="inlineStr">
@@ -8115,6 +8515,21 @@
           <t>Type: Aura Special Rules. Armies: Change Disciples, Wormhole Daemons of Change</t>
         </is>
       </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T113" t="inlineStr">
+        <is>
+          <t>Changebound Boost</t>
+        </is>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="114" ht="40" customHeight="1">
       <c r="A114" s="4" t="inlineStr">
@@ -8251,6 +8666,21 @@
           <t>Type: Defense. Armies: Wormhole Daemons of Change</t>
         </is>
       </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>BOOST</t>
+        </is>
+      </c>
+      <c r="T115" t="inlineStr">
+        <is>
+          <t>Enhances Changebound</t>
+        </is>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>SELF</t>
+        </is>
+      </c>
     </row>
     <row r="116" ht="40" customHeight="1">
       <c r="A116" s="4" t="inlineStr">
@@ -8305,6 +8735,21 @@
       <c r="R116" s="5" t="inlineStr">
         <is>
           <t>Type: Unit. Armies: Change Disciples, Wormhole Daemons of Change</t>
+        </is>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T116" t="inlineStr">
+        <is>
+          <t>Changebound Boost</t>
+        </is>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -8431,6 +8876,21 @@
           <t>Type: Aura Special Rules. Armies: Eternal Dynasty</t>
         </is>
       </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T118" t="inlineStr">
+        <is>
+          <t>Clan Warrior Boost</t>
+        </is>
+      </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="119" ht="40" customHeight="1">
       <c r="A119" s="4" t="inlineStr">
@@ -8559,6 +9019,21 @@
           <t>Type: Aura Special Rules. Armies: Lust Disciples, Wormhole Daemons of Lust</t>
         </is>
       </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T120" t="inlineStr">
+        <is>
+          <t>Quick Shot</t>
+        </is>
+      </c>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="121" ht="40" customHeight="1">
       <c r="A121" s="4" t="inlineStr">
@@ -8851,6 +9326,21 @@
           <t>Type: Aura Special Rules. Armies: DAO Union, Eternal Dynasty, Saurian Starhost, Wolf Brothers, Wolf Prime Brothers (+1 more)</t>
         </is>
       </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T125" t="inlineStr">
+        <is>
+          <t>Counter-Attack</t>
+        </is>
+      </c>
+      <c r="U125" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="126" ht="40" customHeight="1">
       <c r="A126" s="4" t="inlineStr">
@@ -8917,6 +9407,21 @@
       <c r="R126" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Blessed Sisters, Blood Brothers, Blood Prime Brothers, Dark Brothers (+11 more)</t>
+        </is>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T126" t="inlineStr">
+        <is>
+          <t>+1 to morale test rolls</t>
+        </is>
+      </c>
+      <c r="U126" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -9191,6 +9696,21 @@
           <t>Type: Aura Special Rules. Armies: High Elf Fleets</t>
         </is>
       </c>
+      <c r="S130" t="inlineStr">
+        <is>
+          <t>DEBUFF</t>
+        </is>
+      </c>
+      <c r="T130" t="inlineStr">
+        <is>
+          <t>Unwieldy</t>
+        </is>
+      </c>
+      <c r="U130" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="131" ht="40" customHeight="1">
       <c r="A131" s="4" t="inlineStr">
@@ -9663,6 +10183,21 @@
           <t>Type: Aura Special Rules. Armies: Machine Cult</t>
         </is>
       </c>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T137" t="inlineStr">
+        <is>
+          <t>Hit &amp; Run Shooter</t>
+        </is>
+      </c>
+      <c r="U137" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="138" ht="40" customHeight="1">
       <c r="A138" s="4" t="inlineStr">
@@ -9783,6 +10318,21 @@
           <t>Type: Aura Special Rules. Armies: Havoc Brothers</t>
         </is>
       </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T139" t="inlineStr">
+        <is>
+          <t>Shred in melee</t>
+        </is>
+      </c>
+      <c r="U139" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="140" ht="40" customHeight="1">
       <c r="A140" s="4" t="inlineStr">
@@ -9843,6 +10393,21 @@
           <t>Type: Aura Special Rules. Armies: Dark Brothers, Dark Prime Brothers</t>
         </is>
       </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T140" t="inlineStr">
+        <is>
+          <t>Evasive</t>
+        </is>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="141" ht="40" customHeight="1">
       <c r="A141" s="4" t="inlineStr">
@@ -9901,6 +10466,21 @@
       <c r="R141" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Dark Brothers, Dark Prime Brothers</t>
+        </is>
+      </c>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T141" t="inlineStr">
+        <is>
+          <t>Unstoppable</t>
+        </is>
+      </c>
+      <c r="U141" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -10699,6 +11279,21 @@
           <t>Type: Aura Special Rules. Armies: Human Inquisition</t>
         </is>
       </c>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T153" t="inlineStr">
+        <is>
+          <t>Defensive Growth</t>
+        </is>
+      </c>
+      <c r="U153" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="154" ht="40" customHeight="1">
       <c r="A154" s="4" t="inlineStr">
@@ -11155,6 +11750,21 @@
           <t>Type: Weapon. Armies: Blessed Sisters</t>
         </is>
       </c>
+      <c r="S160" t="inlineStr">
+        <is>
+          <t>BOOST</t>
+        </is>
+      </c>
+      <c r="T160" t="inlineStr">
+        <is>
+          <t>Enhances Devout</t>
+        </is>
+      </c>
+      <c r="U160" t="inlineStr">
+        <is>
+          <t>SELF</t>
+        </is>
+      </c>
     </row>
     <row r="161" ht="40" customHeight="1">
       <c r="A161" s="4" t="inlineStr">
@@ -11207,6 +11817,21 @@
           <t>Type: Aura Special Rules. Armies: Blessed Sisters</t>
         </is>
       </c>
+      <c r="S161" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T161" t="inlineStr">
+        <is>
+          <t>Devout Boost</t>
+        </is>
+      </c>
+      <c r="U161" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="162" ht="40" customHeight="1">
       <c r="A162" s="4" t="inlineStr">
@@ -11603,6 +12228,21 @@
           <t>Type: Aura Special Rules. Armies: Orc Marauders</t>
         </is>
       </c>
+      <c r="S167" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T167" t="inlineStr">
+        <is>
+          <t>Resistance</t>
+        </is>
+      </c>
+      <c r="U167" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="168" ht="40" customHeight="1">
       <c r="A168" s="4" t="inlineStr">
@@ -11799,6 +12439,21 @@
           <t>Type: Aura Special Rules. Armies: Ratmen Clans</t>
         </is>
       </c>
+      <c r="S170" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T170" t="inlineStr">
+        <is>
+          <t>Regeneration</t>
+        </is>
+      </c>
+      <c r="U170" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="171" ht="40" customHeight="1">
       <c r="A171" s="4" t="inlineStr">
@@ -11859,6 +12514,21 @@
           <t>Type: Defense. Armies: Human Defense Force</t>
         </is>
       </c>
+      <c r="S171" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T171" t="inlineStr">
+        <is>
+          <t>Entrenched</t>
+        </is>
+      </c>
+      <c r="U171" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="172" ht="40" customHeight="1">
       <c r="A172" s="4" t="inlineStr">
@@ -12111,6 +12781,21 @@
           <t>Type: Aura Special Rules. Armies: Ratmen Clans</t>
         </is>
       </c>
+      <c r="S175" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T175" t="inlineStr">
+        <is>
+          <t>Evasive</t>
+        </is>
+      </c>
+      <c r="U175" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="176" ht="40" customHeight="1">
       <c r="A176" s="4" t="inlineStr">
@@ -12289,6 +12974,21 @@
       <c r="R178" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Dark Elf Raiders</t>
+        </is>
+      </c>
+      <c r="S178" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T178" t="inlineStr">
+        <is>
+          <t>Stealth</t>
+        </is>
+      </c>
+      <c r="U178" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -12543,6 +13243,21 @@
           <t>Type: Aura Special Rules. Armies: Saurian Starhost</t>
         </is>
       </c>
+      <c r="S182" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T182" t="inlineStr">
+        <is>
+          <t>Furious</t>
+        </is>
+      </c>
+      <c r="U182" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="183" ht="40" customHeight="1">
       <c r="A183" s="4" t="inlineStr">
@@ -12673,6 +13388,21 @@
       <c r="R184" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Eternal Dynasty, Wormhole Daemons of Change</t>
+        </is>
+      </c>
+      <c r="S184" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T184" t="inlineStr">
+        <is>
+          <t>Fearless</t>
+        </is>
+      </c>
+      <c r="U184" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -12871,6 +13601,21 @@
           <t>Type: Weapon. Armies: Orc Marauders</t>
         </is>
       </c>
+      <c r="S187" t="inlineStr">
+        <is>
+          <t>BOOST</t>
+        </is>
+      </c>
+      <c r="T187" t="inlineStr">
+        <is>
+          <t>Enhances Ferocious</t>
+        </is>
+      </c>
+      <c r="U187" t="inlineStr">
+        <is>
+          <t>SELF</t>
+        </is>
+      </c>
     </row>
     <row r="188" ht="40" customHeight="1">
       <c r="A188" s="4" t="inlineStr">
@@ -12923,6 +13668,21 @@
           <t>Type: Aura Special Rules. Armies: Orc Marauders</t>
         </is>
       </c>
+      <c r="S188" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T188" t="inlineStr">
+        <is>
+          <t>Ferocious Boost</t>
+        </is>
+      </c>
+      <c r="U188" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="189" ht="40" customHeight="1">
       <c r="A189" s="4" t="inlineStr">
@@ -12981,6 +13741,21 @@
       <c r="R189" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: War Disciples, Wormhole Daemons of War</t>
+        </is>
+      </c>
+      <c r="S189" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T189" t="inlineStr">
+        <is>
+          <t>Melee Evasion</t>
+        </is>
+      </c>
+      <c r="U189" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -13171,6 +13946,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers</t>
         </is>
       </c>
+      <c r="S192" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T192" t="inlineStr">
+        <is>
+          <t>Unpredictable Fighter</t>
+        </is>
+      </c>
+      <c r="U192" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="193" ht="40" customHeight="1">
       <c r="A193" s="4" t="inlineStr">
@@ -13363,6 +14153,21 @@
           <t>Type: Aura Special Rules. Armies: Blessed Sisters, DAO Union, Infected Colonies</t>
         </is>
       </c>
+      <c r="S195" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T195" t="inlineStr">
+        <is>
+          <t>Fortified</t>
+        </is>
+      </c>
+      <c r="U195" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="196" ht="40" customHeight="1">
       <c r="A196" s="4" t="inlineStr">
@@ -13651,6 +14456,21 @@
           <t>Type: Aura Special Rules. Armies: Alien Hives, Change Disciples, Dark Elf Raiders, Havoc Brothers, Human Inquisition (+4 more)</t>
         </is>
       </c>
+      <c r="S199" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T199" t="inlineStr">
+        <is>
+          <t>Furious</t>
+        </is>
+      </c>
+      <c r="U199" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="200" ht="40" customHeight="1">
       <c r="A200" s="4" t="inlineStr">
@@ -13711,6 +14531,21 @@
           <t>Type: Weapon. Armies: Rebel Guerrillas</t>
         </is>
       </c>
+      <c r="S200" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T200" t="inlineStr">
+        <is>
+          <t>Furious</t>
+        </is>
+      </c>
+      <c r="U200" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="201" ht="40" customHeight="1">
       <c r="A201" s="4" t="inlineStr">
@@ -13899,6 +14734,21 @@
           <t>Type: Aura Special Rules. Armies: Soul-Snatcher Cults</t>
         </is>
       </c>
+      <c r="S203" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T203" t="inlineStr">
+        <is>
+          <t>Grounded Precision</t>
+        </is>
+      </c>
+      <c r="U203" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="204" ht="40" customHeight="1">
       <c r="A204" s="4" t="inlineStr">
@@ -13951,6 +14801,21 @@
           <t>Type: Aura Special Rules. Armies: Soul-Snatcher Cults</t>
         </is>
       </c>
+      <c r="S204" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T204" t="inlineStr">
+        <is>
+          <t>Grounded Reinforcement</t>
+        </is>
+      </c>
+      <c r="U204" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="205" ht="40" customHeight="1">
       <c r="A205" s="4" t="inlineStr">
@@ -14083,6 +14948,21 @@
           <t>Type: Defense. Armies: Blessed Sisters</t>
         </is>
       </c>
+      <c r="S206" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T206" t="inlineStr">
+        <is>
+          <t>Guarded</t>
+        </is>
+      </c>
+      <c r="U206" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="207" ht="40" customHeight="1">
       <c r="A207" s="4" t="inlineStr">
@@ -14213,6 +15093,21 @@
       <c r="R208" s="5" t="inlineStr">
         <is>
           <t>Type: Defense. Armies: Custodian Brothers</t>
+        </is>
+      </c>
+      <c r="S208" t="inlineStr">
+        <is>
+          <t>BOOST</t>
+        </is>
+      </c>
+      <c r="T208" t="inlineStr">
+        <is>
+          <t>Enhances Guardian</t>
+        </is>
+      </c>
+      <c r="U208" t="inlineStr">
+        <is>
+          <t>SELF</t>
         </is>
       </c>
     </row>
@@ -14267,6 +15162,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers</t>
         </is>
       </c>
+      <c r="S209" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T209" t="inlineStr">
+        <is>
+          <t>Guardian Boost</t>
+        </is>
+      </c>
+      <c r="U209" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="210" ht="40" customHeight="1">
       <c r="A210" s="4" t="inlineStr">
@@ -14327,6 +15237,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers</t>
         </is>
       </c>
+      <c r="S210" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T210" t="inlineStr">
+        <is>
+          <t>Guardian Boost</t>
+        </is>
+      </c>
+      <c r="U210" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="211" ht="40" customHeight="1">
       <c r="A211" s="4" t="inlineStr">
@@ -14443,6 +15368,21 @@
           <t>Type: Aura Special Rules. Armies: Rebel Guerrillas</t>
         </is>
       </c>
+      <c r="S212" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T212" t="inlineStr">
+        <is>
+          <t>Guerrilla Boost</t>
+        </is>
+      </c>
+      <c r="U212" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="213" ht="40" customHeight="1">
       <c r="A213" s="4" t="inlineStr">
@@ -14559,6 +15499,21 @@
           <t>Type: Aura Special Rules. Armies: Dark Elf Raiders</t>
         </is>
       </c>
+      <c r="S214" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T214" t="inlineStr">
+        <is>
+          <t>Harassing Boost</t>
+        </is>
+      </c>
+      <c r="U214" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="215" ht="40" customHeight="1">
       <c r="A215" s="4" t="inlineStr">
@@ -14619,6 +15574,21 @@
           <t>Type: Aura Special Rules. Armies: Havoc Brothers</t>
         </is>
       </c>
+      <c r="S215" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T215" t="inlineStr">
+        <is>
+          <t>Havocbound Boost</t>
+        </is>
+      </c>
+      <c r="U215" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="216" ht="40" customHeight="1">
       <c r="A216" s="4" t="inlineStr">
@@ -14939,6 +15909,21 @@
           <t>Type: Aura Special Rules. Armies: Havoc Brothers</t>
         </is>
       </c>
+      <c r="S220" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T220" t="inlineStr">
+        <is>
+          <t>Havocbound Boost</t>
+        </is>
+      </c>
+      <c r="U220" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="221" ht="40" customHeight="1">
       <c r="A221" s="4" t="inlineStr">
@@ -15069,6 +16054,21 @@
       <c r="R222" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Orc Marauders</t>
+        </is>
+      </c>
+      <c r="S222" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T222" t="inlineStr">
+        <is>
+          <t>Rending in melee</t>
+        </is>
+      </c>
+      <c r="U222" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -15335,6 +16335,21 @@
           <t>Type: Aura Special Rules. Armies: High Elf Fleets</t>
         </is>
       </c>
+      <c r="S226" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T226" t="inlineStr">
+        <is>
+          <t>Unpredictable Shooter</t>
+        </is>
+      </c>
+      <c r="U226" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="227" ht="40" customHeight="1">
       <c r="A227" s="4" t="inlineStr">
@@ -15459,6 +16474,21 @@
           <t>Type: Aura Special Rules. Armies: High Elf Fleets</t>
         </is>
       </c>
+      <c r="S228" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T228" t="inlineStr">
+        <is>
+          <t>Highborn Boost</t>
+        </is>
+      </c>
+      <c r="U228" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="229" ht="40" customHeight="1">
       <c r="A229" s="4" t="inlineStr">
@@ -15571,6 +16601,21 @@
           <t>Type: Aura Special Rules. Armies: Orc Marauders, Wormhole Daemons of Lust</t>
         </is>
       </c>
+      <c r="S230" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T230" t="inlineStr">
+        <is>
+          <t>Hit &amp; Run Fighter</t>
+        </is>
+      </c>
+      <c r="U230" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="231" ht="40" customHeight="1">
       <c r="A231" s="4" t="inlineStr">
@@ -15681,6 +16726,21 @@
       <c r="R232" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Custodian Brothers, DAO Union, High Elf Fleets</t>
+        </is>
+      </c>
+      <c r="S232" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T232" t="inlineStr">
+        <is>
+          <t>Hit &amp; Run Shooter</t>
+        </is>
+      </c>
+      <c r="U232" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -15803,6 +16863,21 @@
           <t>Type: Aura Special Rules. Armies: Alien Hives</t>
         </is>
       </c>
+      <c r="S234" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T234" t="inlineStr">
+        <is>
+          <t>Hive Bond Boost</t>
+        </is>
+      </c>
+      <c r="U234" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="235" ht="40" customHeight="1">
       <c r="A235" s="4" t="inlineStr">
@@ -15991,6 +17066,21 @@
           <t>Type: Aura Special Rules. Armies: Human Defense Force</t>
         </is>
       </c>
+      <c r="S237" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T237" t="inlineStr">
+        <is>
+          <t>Hold the Line Boost</t>
+        </is>
+      </c>
+      <c r="U237" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="238" ht="40" customHeight="1">
       <c r="A238" s="4" t="inlineStr">
@@ -16119,6 +17209,21 @@
           <t>Type: Aura Special Rules. Armies: Blessed Sisters</t>
         </is>
       </c>
+      <c r="S239" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T239" t="inlineStr">
+        <is>
+          <t>Piercing Hunter</t>
+        </is>
+      </c>
+      <c r="U239" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="240" ht="40" customHeight="1">
       <c r="A240" s="4" t="inlineStr">
@@ -16243,6 +17348,21 @@
           <t>Type: Aura Special Rules. Armies: Eternal Dynasty</t>
         </is>
       </c>
+      <c r="S241" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T241" t="inlineStr">
+        <is>
+          <t>Ignores Cover when shooting</t>
+        </is>
+      </c>
+      <c r="U241" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="242" ht="40" customHeight="1">
       <c r="A242" s="4" t="inlineStr">
@@ -16309,6 +17429,21 @@
       <c r="R242" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Dwarf Guilds</t>
+        </is>
+      </c>
+      <c r="S242" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T242" t="inlineStr">
+        <is>
+          <t>Ignores Cover when shooting</t>
+        </is>
+      </c>
+      <c r="U242" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -16483,6 +17618,16 @@
           <t>Type: Aura Special Rules. Armies: Alien Hives, Blessed Sisters, DAO Union, Dwarf Guilds, High Elf Fleets</t>
         </is>
       </c>
+      <c r="S245" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="U245" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="246" ht="40" customHeight="1">
       <c r="A246" s="4" t="inlineStr">
@@ -16545,6 +17690,16 @@
       <c r="R246" s="5" t="inlineStr">
         <is>
           <t>Type: Weapon. Armies: Soul-Snatcher Cults</t>
+        </is>
+      </c>
+      <c r="S246" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="U246" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -16671,6 +17826,21 @@
           <t>Type: Weapon. Armies: Robot Legions</t>
         </is>
       </c>
+      <c r="S248" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T248" t="inlineStr">
+        <is>
+          <t>Indirect</t>
+        </is>
+      </c>
+      <c r="U248" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="249" ht="40" customHeight="1">
       <c r="A249" s="4" t="inlineStr">
@@ -16721,6 +17891,21 @@
       <c r="R249" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Wormhole Daemons of Change</t>
+        </is>
+      </c>
+      <c r="S249" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T249" t="inlineStr">
+        <is>
+          <t>Indirect when shooting</t>
+        </is>
+      </c>
+      <c r="U249" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -16831,6 +18016,21 @@
           <t>Type: Aura Special Rules. Armies: Infected Colonies</t>
         </is>
       </c>
+      <c r="S251" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T251" t="inlineStr">
+        <is>
+          <t>Infected Boost</t>
+        </is>
+      </c>
+      <c r="U251" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="252" ht="40" customHeight="1">
       <c r="A252" s="4" t="inlineStr">
@@ -16967,6 +18167,21 @@
           <t>Type: Aura Special Rules. Armies: Dwarf Guilds</t>
         </is>
       </c>
+      <c r="S253" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T253" t="inlineStr">
+        <is>
+          <t>Infiltrate</t>
+        </is>
+      </c>
+      <c r="U253" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="254" ht="40" customHeight="1">
       <c r="A254" s="4" t="inlineStr">
@@ -17027,6 +18242,21 @@
           <t>Type: Aura Special Rules. Armies: Alien Hives</t>
         </is>
       </c>
+      <c r="S254" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T254" t="inlineStr">
+        <is>
+          <t>Hive Bond Boost</t>
+        </is>
+      </c>
+      <c r="U254" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="255" ht="40" customHeight="1">
       <c r="A255" s="4" t="inlineStr">
@@ -17139,6 +18369,21 @@
           <t>Type: Aura Special Rules. Armies: Soul-Snatcher Cults</t>
         </is>
       </c>
+      <c r="S256" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T256" t="inlineStr">
+        <is>
+          <t>Grounded Reinforcement</t>
+        </is>
+      </c>
+      <c r="U256" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="257" ht="40" customHeight="1">
       <c r="A257" s="4" t="inlineStr">
@@ -17197,6 +18442,21 @@
       <c r="R257" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Robot Legions</t>
+        </is>
+      </c>
+      <c r="S257" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T257" t="inlineStr">
+        <is>
+          <t>Rapid Advance</t>
+        </is>
+      </c>
+      <c r="U257" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -17467,6 +18727,21 @@
           <t>Type: Aura Special Rules. Armies: Knight Brothers, Knight Prime Brothers</t>
         </is>
       </c>
+      <c r="S261" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T261" t="inlineStr">
+        <is>
+          <t>Evasive</t>
+        </is>
+      </c>
+      <c r="U261" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="262" ht="40" customHeight="1">
       <c r="A262" s="4" t="inlineStr">
@@ -17525,6 +18800,21 @@
       <c r="R262" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Knight Brothers, Knight Prime Brothers</t>
+        </is>
+      </c>
+      <c r="S262" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T262" t="inlineStr">
+        <is>
+          <t>Unstoppable</t>
+        </is>
+      </c>
+      <c r="U262" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -17979,6 +19269,21 @@
           <t>Type: Aura Special Rules. Armies: Blessed Sisters</t>
         </is>
       </c>
+      <c r="S269" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T269" t="inlineStr">
+        <is>
+          <t>Devout Boost</t>
+        </is>
+      </c>
+      <c r="U269" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="270" ht="40" customHeight="1">
       <c r="A270" s="4" t="inlineStr">
@@ -18039,6 +19344,21 @@
           <t>Type: Aura Special Rules. Armies: Lust Disciples, Wormhole Daemons of Lust</t>
         </is>
       </c>
+      <c r="S270" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T270" t="inlineStr">
+        <is>
+          <t>Lustbound Boost</t>
+        </is>
+      </c>
+      <c r="U270" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="271" ht="40" customHeight="1">
       <c r="A271" s="4" t="inlineStr">
@@ -18181,6 +19501,21 @@
       <c r="R272" s="5" t="inlineStr">
         <is>
           <t>Type: Movement. Armies: Wormhole Daemons of Lust</t>
+        </is>
+      </c>
+      <c r="S272" t="inlineStr">
+        <is>
+          <t>BOOST</t>
+        </is>
+      </c>
+      <c r="T272" t="inlineStr">
+        <is>
+          <t>Enhances Lustbound</t>
+        </is>
+      </c>
+      <c r="U272" t="inlineStr">
+        <is>
+          <t>SELF</t>
         </is>
       </c>
     </row>
@@ -18235,6 +19570,21 @@
           <t>Type: Aura Special Rules. Armies: Lust Disciples, Wormhole Daemons of Lust</t>
         </is>
       </c>
+      <c r="S273" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T273" t="inlineStr">
+        <is>
+          <t>Lustbound Boost</t>
+        </is>
+      </c>
+      <c r="U273" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="274" ht="40" customHeight="1">
       <c r="A274" s="4" t="inlineStr">
@@ -18355,6 +19705,21 @@
           <t>Type: Aura Special Rules. Armies: Machine Cult</t>
         </is>
       </c>
+      <c r="S275" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T275" t="inlineStr">
+        <is>
+          <t>Machine-Fog Boost</t>
+        </is>
+      </c>
+      <c r="U275" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="276" ht="40" customHeight="1">
       <c r="A276" s="4" t="inlineStr">
@@ -18459,6 +19824,21 @@
           <t>Type: Aura Special Rules. Armies: Eternal Dynasty, Goblin Reclaimers, Ratmen Clans</t>
         </is>
       </c>
+      <c r="S277" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T277" t="inlineStr">
+        <is>
+          <t>Melee Evasion</t>
+        </is>
+      </c>
+      <c r="U277" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="278" ht="40" customHeight="1">
       <c r="A278" s="4" t="inlineStr">
@@ -18511,6 +19891,21 @@
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Blood Brothers, Blood Prime Brothers, DAO Union, Dark Brothers (+10 more)</t>
         </is>
       </c>
+      <c r="S278" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T278" t="inlineStr">
+        <is>
+          <t>Melee Shrouding</t>
+        </is>
+      </c>
+      <c r="U278" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="279" ht="40" customHeight="1">
       <c r="A279" s="4" t="inlineStr">
@@ -18629,6 +20024,21 @@
       <c r="R280" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Soul-Snatcher Cults</t>
+        </is>
+      </c>
+      <c r="S280" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T280" t="inlineStr">
+        <is>
+          <t>Melee Slayer</t>
+        </is>
+      </c>
+      <c r="U280" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -18755,6 +20165,21 @@
           <t>Type: Aura Special Rules. Armies: Robot Legions</t>
         </is>
       </c>
+      <c r="S282" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T282" t="inlineStr">
+        <is>
+          <t>Self-Repair Boost</t>
+        </is>
+      </c>
+      <c r="U282" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="283" ht="40" customHeight="1">
       <c r="A283" s="4" t="inlineStr">
@@ -19331,6 +20756,21 @@
           <t>Type: Aura Special Rules. Armies: Goblin Reclaimers</t>
         </is>
       </c>
+      <c r="S291" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T291" t="inlineStr">
+        <is>
+          <t>Mischievous Boost</t>
+        </is>
+      </c>
+      <c r="U291" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="292" ht="40" customHeight="1">
       <c r="A292" s="4" t="inlineStr">
@@ -19537,6 +20977,21 @@
       <c r="R294" s="5" t="inlineStr">
         <is>
           <t>Type: Defense. Armies: Human Defense Force, Jackals</t>
+        </is>
+      </c>
+      <c r="S294" t="inlineStr">
+        <is>
+          <t>DEBUFF</t>
+        </is>
+      </c>
+      <c r="T294" t="inlineStr">
+        <is>
+          <t>-1 to morale test rolls</t>
+        </is>
+      </c>
+      <c r="U294" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -19651,6 +21106,21 @@
           <t>Type: Aura Special Rules. Armies: Infected Colonies, Robot Legions</t>
         </is>
       </c>
+      <c r="S296" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T296" t="inlineStr">
+        <is>
+          <t>No Retreat</t>
+        </is>
+      </c>
+      <c r="U296" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="297" ht="40" customHeight="1">
       <c r="A297" s="4" t="inlineStr">
@@ -19711,6 +21181,21 @@
           <t>Type: Defense. Armies: Human Defense Force</t>
         </is>
       </c>
+      <c r="S297" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T297" t="inlineStr">
+        <is>
+          <t>No Retreat</t>
+        </is>
+      </c>
+      <c r="U297" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="298" ht="40" customHeight="1">
       <c r="A298" s="4" t="inlineStr">
@@ -19907,6 +21392,21 @@
           <t>Type: Aura Special Rules. Armies: Orc Marauders</t>
         </is>
       </c>
+      <c r="S300" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T300" t="inlineStr">
+        <is>
+          <t>Ferocious Boost</t>
+        </is>
+      </c>
+      <c r="U300" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="301" ht="40" customHeight="1">
       <c r="A301" s="4" t="inlineStr">
@@ -19959,6 +21459,21 @@
           <t>Type: Aura Special Rules. Armies: Blood Brothers, Blood Prime Brothers, Ratmen Clans, Robot Legions, Wormhole Daemons of Lust</t>
         </is>
       </c>
+      <c r="S301" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T301" t="inlineStr">
+        <is>
+          <t>Piercing Assault</t>
+        </is>
+      </c>
+      <c r="U301" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="302" ht="40" customHeight="1">
       <c r="A302" s="4" t="inlineStr">
@@ -20095,6 +21610,16 @@
           <t>Type: Aura Special Rules. Armies: Orc Marauders, Wormhole Daemons of War</t>
         </is>
       </c>
+      <c r="S303" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="U303" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="304" ht="40" customHeight="1">
       <c r="A304" s="4" t="inlineStr">
@@ -20223,6 +21748,21 @@
           <t>Type: Aura Special Rules. Armies: Dark Elf Raiders, Eternal Dynasty</t>
         </is>
       </c>
+      <c r="S305" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T305" t="inlineStr">
+        <is>
+          <t>Piercing Hunter</t>
+        </is>
+      </c>
+      <c r="U305" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="306" ht="40" customHeight="1">
       <c r="A306" s="4" t="inlineStr">
@@ -20359,6 +21899,16 @@
           <t>Type: Aura Special Rules. Armies: Wormhole Daemons of War</t>
         </is>
       </c>
+      <c r="S307" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="U307" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="308" ht="40" customHeight="1">
       <c r="A308" s="4" t="inlineStr">
@@ -20823,6 +22373,21 @@
           <t>Type: Aura Special Rules. Armies: Plague Disciples, Wormhole Daemons of Plague</t>
         </is>
       </c>
+      <c r="S314" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T314" t="inlineStr">
+        <is>
+          <t>Plaguebound Boost</t>
+        </is>
+      </c>
+      <c r="U314" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="315" ht="40" customHeight="1">
       <c r="A315" s="4" t="inlineStr">
@@ -21035,6 +22600,21 @@
           <t>Type: Defense. Armies: Wormhole Daemons of Plague</t>
         </is>
       </c>
+      <c r="S317" t="inlineStr">
+        <is>
+          <t>BOOST</t>
+        </is>
+      </c>
+      <c r="T317" t="inlineStr">
+        <is>
+          <t>Enhances Plaguebound</t>
+        </is>
+      </c>
+      <c r="U317" t="inlineStr">
+        <is>
+          <t>SELF</t>
+        </is>
+      </c>
     </row>
     <row r="318" ht="40" customHeight="1">
       <c r="A318" s="4" t="inlineStr">
@@ -21087,6 +22667,21 @@
           <t>Type: Aura Special Rules. Armies: Plague Disciples, Wormhole Daemons of Plague</t>
         </is>
       </c>
+      <c r="S318" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T318" t="inlineStr">
+        <is>
+          <t>Plaguebound Boost</t>
+        </is>
+      </c>
+      <c r="U318" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="319" ht="40" customHeight="1">
       <c r="A319" s="4" t="inlineStr">
@@ -21139,6 +22734,21 @@
           <t>Type: Aura Special Rules. Armies: Blessed Sisters</t>
         </is>
       </c>
+      <c r="S319" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T319" t="inlineStr">
+        <is>
+          <t>Point-Blank Piercing</t>
+        </is>
+      </c>
+      <c r="U319" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="320" ht="40" customHeight="1">
       <c r="A320" s="4" t="inlineStr">
@@ -21403,6 +23013,21 @@
           <t>Type: Aura Special Rules. Armies: Jackals</t>
         </is>
       </c>
+      <c r="S323" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T323" t="inlineStr">
+        <is>
+          <t>Shielded</t>
+        </is>
+      </c>
+      <c r="U323" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="324" ht="40" customHeight="1">
       <c r="A324" s="4" t="inlineStr">
@@ -21675,6 +23300,21 @@
           <t>Type: Aura Special Rules. Armies: Orc Marauders</t>
         </is>
       </c>
+      <c r="S327" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T327" t="inlineStr">
+        <is>
+          <t>+1 to hit rolls when charging</t>
+        </is>
+      </c>
+      <c r="U327" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="328" ht="40" customHeight="1">
       <c r="A328" s="4" t="inlineStr">
@@ -21811,6 +23451,21 @@
           <t>Type: Aura Special Rules. Armies: Eternal Dynasty, Goblin Reclaimers, Human Inquisition, Jackals</t>
         </is>
       </c>
+      <c r="S329" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T329" t="inlineStr">
+        <is>
+          <t>+1 to hit rolls in melee</t>
+        </is>
+      </c>
+      <c r="U329" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="330" ht="40" customHeight="1">
       <c r="A330" s="4" t="inlineStr">
@@ -22097,6 +23752,21 @@
       <c r="R333" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Human Inquisition, Ratmen Clans</t>
+        </is>
+      </c>
+      <c r="S333" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T333" t="inlineStr">
+        <is>
+          <t>+1 to hit rolls when shooting</t>
+        </is>
+      </c>
+      <c r="U333" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -22563,6 +24233,21 @@
           <t>Type: Weapon. Armies: Saurian Starhost</t>
         </is>
       </c>
+      <c r="S340" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T340" t="inlineStr">
+        <is>
+          <t>Primal Boost</t>
+        </is>
+      </c>
+      <c r="U340" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="341" ht="40" customHeight="1">
       <c r="A341" s="4" t="inlineStr">
@@ -22695,6 +24380,21 @@
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Prime Brothers</t>
         </is>
       </c>
+      <c r="S342" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T342" t="inlineStr">
+        <is>
+          <t>Evasive</t>
+        </is>
+      </c>
+      <c r="U342" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="343" ht="40" customHeight="1">
       <c r="A343" s="4" t="inlineStr">
@@ -22755,6 +24455,21 @@
           <t>Type: Aura Special Rules. Armies: Dark Elf Raiders</t>
         </is>
       </c>
+      <c r="S343" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T343" t="inlineStr">
+        <is>
+          <t>Harassing Boost</t>
+        </is>
+      </c>
+      <c r="U343" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="344" ht="40" customHeight="1">
       <c r="A344" s="4" t="inlineStr">
@@ -22883,6 +24598,21 @@
           <t>Type: Aura Special Rules. Armies: Jackals</t>
         </is>
       </c>
+      <c r="S345" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T345" t="inlineStr">
+        <is>
+          <t>Scrapper Boost</t>
+        </is>
+      </c>
+      <c r="U345" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="346" ht="40" customHeight="1">
       <c r="A346" s="4" t="inlineStr">
@@ -22943,6 +24673,21 @@
           <t>Type: Aura Special Rules. Armies: Human Defense Force, Human Inquisition, Titan Lords</t>
         </is>
       </c>
+      <c r="S346" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T346" t="inlineStr">
+        <is>
+          <t>Hold the Line Boost</t>
+        </is>
+      </c>
+      <c r="U346" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="347" ht="40" customHeight="1">
       <c r="A347" s="4" t="inlineStr">
@@ -23139,6 +24884,21 @@
           <t>Type: Aura Special Rules. Armies: DAO Union</t>
         </is>
       </c>
+      <c r="S349" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T349" t="inlineStr">
+        <is>
+          <t>Targeting Visor Boost</t>
+        </is>
+      </c>
+      <c r="U349" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="350" ht="40" customHeight="1">
       <c r="A350" s="4" t="inlineStr">
@@ -23643,6 +25403,21 @@
           <t>Type: Aura Special Rules. Armies: Goblin Reclaimers, Soul-Snatcher Cults</t>
         </is>
       </c>
+      <c r="S357" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T357" t="inlineStr">
+        <is>
+          <t>Quick Shot</t>
+        </is>
+      </c>
+      <c r="U357" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="358" ht="40" customHeight="1">
       <c r="A358" s="4" t="inlineStr">
@@ -23703,6 +25478,21 @@
           <t>Type: Weapon. Armies: Wormhole Daemons of Lust</t>
         </is>
       </c>
+      <c r="S358" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T358" t="inlineStr">
+        <is>
+          <t>Quick Shot</t>
+        </is>
+      </c>
+      <c r="U358" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="359" ht="40" customHeight="1">
       <c r="A359" s="4" t="inlineStr">
@@ -23891,6 +25681,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers, Jackals, Orc Marauders</t>
         </is>
       </c>
+      <c r="S361" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T361" t="inlineStr">
+        <is>
+          <t>Ranged Shrouding</t>
+        </is>
+      </c>
+      <c r="U361" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="362" ht="40" customHeight="1">
       <c r="A362" s="4" t="inlineStr">
@@ -23941,6 +25746,21 @@
       <c r="R362" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: DAO Union</t>
+        </is>
+      </c>
+      <c r="S362" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T362" t="inlineStr">
+        <is>
+          <t>Ranged Slayer</t>
+        </is>
+      </c>
+      <c r="U362" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -23995,6 +25815,21 @@
           <t>Type: Aura Special Rules. Armies: Eternal Dynasty</t>
         </is>
       </c>
+      <c r="S363" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T363" t="inlineStr">
+        <is>
+          <t>Rapid Advance</t>
+        </is>
+      </c>
+      <c r="U363" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="364" ht="40" customHeight="1">
       <c r="A364" s="4" t="inlineStr">
@@ -24057,6 +25892,21 @@
       <c r="R364" s="5" t="inlineStr">
         <is>
           <t>Type: Movement. Armies: Human Defense Force</t>
+        </is>
+      </c>
+      <c r="S364" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T364" t="inlineStr">
+        <is>
+          <t>Rapid Advance</t>
+        </is>
+      </c>
+      <c r="U364" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -24239,6 +26089,21 @@
           <t>Type: Aura Special Rules. Armies: Elven Jesters</t>
         </is>
       </c>
+      <c r="S367" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T367" t="inlineStr">
+        <is>
+          <t>Rapid Blink Boost</t>
+        </is>
+      </c>
+      <c r="U367" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="368" ht="40" customHeight="1">
       <c r="A368" s="4" t="inlineStr">
@@ -24371,6 +26236,21 @@
           <t>Type: Aura Special Rules. Armies: Infected Colonies</t>
         </is>
       </c>
+      <c r="S369" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T369" t="inlineStr">
+        <is>
+          <t>Regeneration</t>
+        </is>
+      </c>
+      <c r="U369" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="370" ht="40" customHeight="1">
       <c r="A370" s="4" t="inlineStr">
@@ -24491,6 +26371,21 @@
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Blood Brothers, Blood Prime Brothers, Dark Brothers, Dark Prime Brothers (+7 more)</t>
         </is>
       </c>
+      <c r="S371" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T371" t="inlineStr">
+        <is>
+          <t>Rapid Rush</t>
+        </is>
+      </c>
+      <c r="U371" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="372" ht="40" customHeight="1">
       <c r="A372" s="4" t="inlineStr">
@@ -24715,6 +26610,21 @@
           <t>Type: Aura Special Rules. Armies: Robot Legions</t>
         </is>
       </c>
+      <c r="S375" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T375" t="inlineStr">
+        <is>
+          <t>Reanimation</t>
+        </is>
+      </c>
+      <c r="U375" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="376" ht="40" customHeight="1">
       <c r="A376" s="4" t="inlineStr">
@@ -24839,6 +26749,21 @@
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Blessed Sisters, Blood Brothers, Blood Prime Brothers, Custodian Brothers (+18 more)</t>
         </is>
       </c>
+      <c r="S377" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T377" t="inlineStr">
+        <is>
+          <t>Regeneration</t>
+        </is>
+      </c>
+      <c r="U377" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="378" ht="40" customHeight="1">
       <c r="A378" s="4" t="inlineStr">
@@ -24899,6 +26824,21 @@
           <t>Type: Defense. Armies: Dark Elf Raiders, Wormhole Daemons of Plague</t>
         </is>
       </c>
+      <c r="S378" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T378" t="inlineStr">
+        <is>
+          <t>Regeneration</t>
+        </is>
+      </c>
+      <c r="U378" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="379" ht="40" customHeight="1">
       <c r="A379" s="4" t="inlineStr">
@@ -25175,6 +27115,21 @@
           <t>Type: Aura Special Rules. Armies: Change Disciples, Havoc Brothers, Lust Disciples, Plague Disciples, Robot Legions (+2 more)</t>
         </is>
       </c>
+      <c r="S382" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T382" t="inlineStr">
+        <is>
+          <t>Relentless</t>
+        </is>
+      </c>
+      <c r="U382" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="383" ht="40" customHeight="1">
       <c r="A383" s="4" t="inlineStr">
@@ -25235,6 +27190,21 @@
           <t>Type: Weapon. Armies: Human Defense Force</t>
         </is>
       </c>
+      <c r="S383" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T383" t="inlineStr">
+        <is>
+          <t>Relentless</t>
+        </is>
+      </c>
+      <c r="U383" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="384" ht="40" customHeight="1">
       <c r="A384" s="4" t="inlineStr">
@@ -25287,6 +27257,21 @@
           <t>Type: Aura Special Rules. Armies: Rebel Guerrillas, Wormhole Daemons of Plague</t>
         </is>
       </c>
+      <c r="S384" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T384" t="inlineStr">
+        <is>
+          <t>Rending in melee</t>
+        </is>
+      </c>
+      <c r="U384" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="385" ht="40" customHeight="1">
       <c r="A385" s="4" t="inlineStr">
@@ -25351,6 +27336,21 @@
           <t>Type: Weapon. Armies: Orc Marauders</t>
         </is>
       </c>
+      <c r="S385" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T385" t="inlineStr">
+        <is>
+          <t>Rending in melee</t>
+        </is>
+      </c>
+      <c r="U385" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="386" ht="40" customHeight="1">
       <c r="A386" s="4" t="inlineStr">
@@ -25401,6 +27401,21 @@
       <c r="R386" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Machine Cult, Saurian Starhost</t>
+        </is>
+      </c>
+      <c r="S386" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T386" t="inlineStr">
+        <is>
+          <t>Rending when shooting</t>
+        </is>
+      </c>
+      <c r="U386" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -25523,6 +27538,21 @@
           <t>Type: Aura Special Rules. Armies: Change Disciples, Havoc Brothers, High Elf Fleets, Human Inquisition, Lust Disciples (+3 more)</t>
         </is>
       </c>
+      <c r="S388" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T388" t="inlineStr">
+        <is>
+          <t>Resistance</t>
+        </is>
+      </c>
+      <c r="U388" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="389" ht="40" customHeight="1">
       <c r="A389" s="4" t="inlineStr">
@@ -25643,6 +27673,21 @@
           <t>Type: Aura Special Rules. Armies: Wolf Brothers, Wolf Prime Brothers</t>
         </is>
       </c>
+      <c r="S390" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T390" t="inlineStr">
+        <is>
+          <t>Piercing Assault</t>
+        </is>
+      </c>
+      <c r="U390" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="391" ht="40" customHeight="1">
       <c r="A391" s="4" t="inlineStr">
@@ -25915,6 +27960,21 @@
           <t>Type: Aura Special Rules. Armies: Change Disciples, Havoc Brothers, High Elf Fleets, Jackals, Lust Disciples (+3 more)</t>
         </is>
       </c>
+      <c r="S394" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T394" t="inlineStr">
+        <is>
+          <t>Scout</t>
+        </is>
+      </c>
+      <c r="U394" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="395" ht="40" customHeight="1">
       <c r="A395" s="4" t="inlineStr">
@@ -26023,6 +28083,21 @@
           <t>Type: Aura Special Rules. Armies: Jackals</t>
         </is>
       </c>
+      <c r="S396" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T396" t="inlineStr">
+        <is>
+          <t>Scrapper Boost</t>
+        </is>
+      </c>
+      <c r="U396" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="397" ht="40" customHeight="1">
       <c r="A397" s="4" t="inlineStr">
@@ -26219,6 +28294,21 @@
           <t>Type: Aura Special Rules. Armies: Ratmen Clans</t>
         </is>
       </c>
+      <c r="S399" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T399" t="inlineStr">
+        <is>
+          <t>Scurry Boost</t>
+        </is>
+      </c>
+      <c r="U399" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="400" ht="40" customHeight="1">
       <c r="A400" s="4" t="inlineStr">
@@ -26615,6 +28705,21 @@
           <t>Type: Defense. Armies: Robot Legions</t>
         </is>
       </c>
+      <c r="S405" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T405" t="inlineStr">
+        <is>
+          <t>Self-Repair Boost</t>
+        </is>
+      </c>
+      <c r="U405" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="406" ht="40" customHeight="1">
       <c r="A406" s="4" t="inlineStr">
@@ -26743,6 +28848,21 @@
           <t>Type: Aura Special Rules. Armies: Elven Jesters</t>
         </is>
       </c>
+      <c r="S407" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T407" t="inlineStr">
+        <is>
+          <t>Rapid Blink Boost</t>
+        </is>
+      </c>
+      <c r="U407" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="408" ht="40" customHeight="1">
       <c r="A408" s="4" t="inlineStr">
@@ -27019,6 +29139,21 @@
           <t>Type: Aura Special Rules. Armies: Alien Hives, Elven Jesters, Wormhole Daemons of War</t>
         </is>
       </c>
+      <c r="S411" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T411" t="inlineStr">
+        <is>
+          <t>Shielded</t>
+        </is>
+      </c>
+      <c r="U411" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="412" ht="40" customHeight="1">
       <c r="A412" s="4" t="inlineStr">
@@ -27079,6 +29214,21 @@
           <t>Type: Aura Special Rules. Armies: Change Disciples, Wormhole Daemons of Change</t>
         </is>
       </c>
+      <c r="S412" t="inlineStr">
+        <is>
+          <t>DEBUFF</t>
+        </is>
+      </c>
+      <c r="T412" t="inlineStr">
+        <is>
+          <t>-3 to casting rolls</t>
+        </is>
+      </c>
+      <c r="U412" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="413" ht="40" customHeight="1">
       <c r="A413" s="4" t="inlineStr">
@@ -27211,6 +29361,21 @@
           <t>Type: Weapon. Armies: Custodian Brothers</t>
         </is>
       </c>
+      <c r="S414" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T414" t="inlineStr">
+        <is>
+          <t>Shred</t>
+        </is>
+      </c>
+      <c r="U414" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="415" ht="40" customHeight="1">
       <c r="A415" s="4" t="inlineStr">
@@ -27263,6 +29428,21 @@
           <t>Type: Aura Special Rules. Armies: Blessed Sisters, High Elf Fleets, Human Inquisition</t>
         </is>
       </c>
+      <c r="S415" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T415" t="inlineStr">
+        <is>
+          <t>Shred in melee</t>
+        </is>
+      </c>
+      <c r="U415" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="416" ht="40" customHeight="1">
       <c r="A416" s="4" t="inlineStr">
@@ -27313,6 +29493,21 @@
       <c r="R416" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Custodian Brothers, Elven Jesters, Watch Brothers, Watch Prime Brothers</t>
+        </is>
+      </c>
+      <c r="S416" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T416" t="inlineStr">
+        <is>
+          <t>Shred when shooting</t>
+        </is>
+      </c>
+      <c r="U416" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -27443,6 +29638,21 @@
           <t>Type: Aura Special Rules. Armies: Machine Cult</t>
         </is>
       </c>
+      <c r="S418" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T418" t="inlineStr">
+        <is>
+          <t>Machine-Fog Boost</t>
+        </is>
+      </c>
+      <c r="U418" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="419" ht="40" customHeight="1">
       <c r="A419" s="4" t="inlineStr">
@@ -27775,6 +29985,21 @@
           <t>Type: Weapon. Armies: Elven Jesters</t>
         </is>
       </c>
+      <c r="S423" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T423" t="inlineStr">
+        <is>
+          <t>Slayer</t>
+        </is>
+      </c>
+      <c r="U423" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="424" ht="40" customHeight="1">
       <c r="A424" s="4" t="inlineStr">
@@ -28231,6 +30456,21 @@
           <t>Type: Aura Special Rules. Armies: Orc Marauders</t>
         </is>
       </c>
+      <c r="S430" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T430" t="inlineStr">
+        <is>
+          <t>Speed Feat</t>
+        </is>
+      </c>
+      <c r="U430" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="431" ht="40" customHeight="1">
       <c r="A431" s="4" t="inlineStr">
@@ -28399,6 +30639,21 @@
           <t>Type: Aura Special Rules. Armies: Eternal Dynasty</t>
         </is>
       </c>
+      <c r="S433" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T433" t="inlineStr">
+        <is>
+          <t>Flying</t>
+        </is>
+      </c>
+      <c r="U433" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="434" ht="40" customHeight="1">
       <c r="A434" s="4" t="inlineStr">
@@ -28459,6 +30714,21 @@
           <t>Type: Aura Special Rules. Armies: Eternal Dynasty</t>
         </is>
       </c>
+      <c r="S434" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T434" t="inlineStr">
+        <is>
+          <t>Clan Warrior Boost</t>
+        </is>
+      </c>
+      <c r="U434" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="435" ht="40" customHeight="1">
       <c r="A435" s="4" t="inlineStr">
@@ -28691,6 +30961,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers, Wormhole Daemons of Plague</t>
         </is>
       </c>
+      <c r="S438" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T438" t="inlineStr">
+        <is>
+          <t>Steadfast</t>
+        </is>
+      </c>
+      <c r="U438" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="439" ht="40" customHeight="1">
       <c r="A439" s="4" t="inlineStr">
@@ -28753,6 +31038,21 @@
       <c r="R439" s="5" t="inlineStr">
         <is>
           <t>Type: Defense. Armies: Change Disciples, Havoc Brothers, Lust Disciples, Plague Disciples, War Disciples</t>
+        </is>
+      </c>
+      <c r="S439" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T439" t="inlineStr">
+        <is>
+          <t>Steadfast</t>
+        </is>
+      </c>
+      <c r="U439" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
         </is>
       </c>
     </row>
@@ -28807,6 +31107,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers, DAO Union, Dwarf Guilds, Eternal Dynasty, High Elf Fleets (+2 more)</t>
         </is>
       </c>
+      <c r="S440" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T440" t="inlineStr">
+        <is>
+          <t>Stealth</t>
+        </is>
+      </c>
+      <c r="U440" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="441" ht="40" customHeight="1">
       <c r="A441" s="4" t="inlineStr">
@@ -28867,6 +31182,21 @@
           <t>Type: Defense. Armies: Alien Hives, Dark Brothers</t>
         </is>
       </c>
+      <c r="S441" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T441" t="inlineStr">
+        <is>
+          <t>Stealth</t>
+        </is>
+      </c>
+      <c r="U441" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="442" ht="40" customHeight="1">
       <c r="A442" s="4" t="inlineStr">
@@ -29359,6 +31689,21 @@
           <t>Type: Aura Special Rules. Armies: Rebel Guerrillas, Wormhole Daemons of Lust</t>
         </is>
       </c>
+      <c r="S448" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T448" t="inlineStr">
+        <is>
+          <t>Strider</t>
+        </is>
+      </c>
+      <c r="U448" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="449" ht="40" customHeight="1">
       <c r="A449" s="4" t="inlineStr">
@@ -29479,6 +31824,21 @@
           <t>Type: Aura Special Rules. Armies: Dwarf Guilds</t>
         </is>
       </c>
+      <c r="S450" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T450" t="inlineStr">
+        <is>
+          <t>Sturdy Boost</t>
+        </is>
+      </c>
+      <c r="U450" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="451" ht="40" customHeight="1">
       <c r="A451" s="4" t="inlineStr">
@@ -29727,6 +32087,21 @@
           <t>Type: Aura Special Rules. Armies: Dwarf Guilds</t>
         </is>
       </c>
+      <c r="S454" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T454" t="inlineStr">
+        <is>
+          <t>Swift</t>
+        </is>
+      </c>
+      <c r="U454" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="455" ht="40" customHeight="1">
       <c r="A455" s="4" t="inlineStr">
@@ -29787,6 +32162,21 @@
           <t>Type: Movement. Armies: Robot Legions</t>
         </is>
       </c>
+      <c r="S455" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T455" t="inlineStr">
+        <is>
+          <t>Swift</t>
+        </is>
+      </c>
+      <c r="U455" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="456" ht="40" customHeight="1">
       <c r="A456" s="4" t="inlineStr">
@@ -30043,6 +32433,21 @@
           <t>Type: Aura Special Rules. Armies: DAO Union</t>
         </is>
       </c>
+      <c r="S459" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T459" t="inlineStr">
+        <is>
+          <t>Targeting Visor Boost</t>
+        </is>
+      </c>
+      <c r="U459" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="460" ht="40" customHeight="1">
       <c r="A460" s="4" t="inlineStr">
@@ -30287,6 +32692,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers, Elven Jesters, Machine Cult, Wormhole Daemons of Change</t>
         </is>
       </c>
+      <c r="S463" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T463" t="inlineStr">
+        <is>
+          <t>Teleport</t>
+        </is>
+      </c>
+      <c r="U463" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="464" ht="40" customHeight="1">
       <c r="A464" s="4" t="inlineStr">
@@ -30405,6 +32825,21 @@
       <c r="R465" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Alien Hives</t>
+        </is>
+      </c>
+      <c r="S465" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T465" t="inlineStr">
+        <is>
+          <t>Unpredictable Fighter</t>
+        </is>
+      </c>
+      <c r="U465" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -30467,6 +32902,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers</t>
         </is>
       </c>
+      <c r="S466" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T466" t="inlineStr">
+        <is>
+          <t>Shred</t>
+        </is>
+      </c>
+      <c r="U466" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="467" ht="40" customHeight="1">
       <c r="A467" s="4" t="inlineStr">
@@ -30585,6 +33035,21 @@
       <c r="R468" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Infected Colonies</t>
+        </is>
+      </c>
+      <c r="S468" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T468" t="inlineStr">
+        <is>
+          <t>Thrust in melee</t>
+        </is>
+      </c>
+      <c r="U468" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
         </is>
       </c>
     </row>
@@ -30783,6 +33248,21 @@
           <t>Type: Aura Special Rules. Armies: Saurian Starhost</t>
         </is>
       </c>
+      <c r="S471" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T471" t="inlineStr">
+        <is>
+          <t>Bane</t>
+        </is>
+      </c>
+      <c r="U471" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="472" ht="40" customHeight="1">
       <c r="A472" s="4" t="inlineStr">
@@ -30841,6 +33321,21 @@
       <c r="R472" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Robot Legions</t>
+        </is>
+      </c>
+      <c r="S472" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T472" t="inlineStr">
+        <is>
+          <t>Indirect</t>
+        </is>
+      </c>
+      <c r="U472" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -31035,6 +33530,21 @@
           <t>Type: Aura Special Rules. Armies: Dwarf Guilds, Elven Jesters, Knight Brothers, Knight Prime Brothers, Machine Cult</t>
         </is>
       </c>
+      <c r="S475" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T475" t="inlineStr">
+        <is>
+          <t>Unpredictable Fighter</t>
+        </is>
+      </c>
+      <c r="U475" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="476" ht="40" customHeight="1">
       <c r="A476" s="4" t="inlineStr">
@@ -31099,6 +33609,21 @@
           <t>Type: Weapon. Armies: Alien Hives</t>
         </is>
       </c>
+      <c r="S476" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T476" t="inlineStr">
+        <is>
+          <t>Unpredictable Fighter</t>
+        </is>
+      </c>
+      <c r="U476" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="477" ht="40" customHeight="1">
       <c r="A477" s="4" t="inlineStr">
@@ -31219,6 +33744,21 @@
           <t>Type: Aura Special Rules. Armies: Infected Colonies, Jackals, Orc Marauders</t>
         </is>
       </c>
+      <c r="S478" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T478" t="inlineStr">
+        <is>
+          <t>Unpredictable Shooter</t>
+        </is>
+      </c>
+      <c r="U478" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="479" ht="40" customHeight="1">
       <c r="A479" s="4" t="inlineStr">
@@ -31281,6 +33821,21 @@
       <c r="R479" s="5" t="inlineStr">
         <is>
           <t>Type: Weapon. Armies: Battle Brothers, Blood Brothers, Blood Prime Brothers, Dark Brothers, Dark Prime Brothers (+7 more)</t>
+        </is>
+      </c>
+      <c r="S479" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T479" t="inlineStr">
+        <is>
+          <t>Unstoppable</t>
+        </is>
+      </c>
+      <c r="U479" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -31335,6 +33890,21 @@
           <t>Type: Aura Special Rules. Armies: Custodian Brothers, Wormhole Daemons of Change</t>
         </is>
       </c>
+      <c r="S480" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T480" t="inlineStr">
+        <is>
+          <t>Unstoppable in melee</t>
+        </is>
+      </c>
+      <c r="U480" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="481" ht="40" customHeight="1">
       <c r="A481" s="4" t="inlineStr">
@@ -31387,6 +33957,21 @@
           <t>Type: Aura Special Rules. Armies: Wormhole Daemons of Lust</t>
         </is>
       </c>
+      <c r="S481" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T481" t="inlineStr">
+        <is>
+          <t>Unstoppable when shooting</t>
+        </is>
+      </c>
+      <c r="U481" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="482" ht="40" customHeight="1">
       <c r="A482" s="4" t="inlineStr">
@@ -31449,6 +34034,21 @@
       <c r="R482" s="5" t="inlineStr">
         <is>
           <t>Type: Defense. Armies: High Elf Fleets</t>
+        </is>
+      </c>
+      <c r="S482" t="inlineStr">
+        <is>
+          <t>DEBUFF</t>
+        </is>
+      </c>
+      <c r="T482" t="inlineStr">
+        <is>
+          <t>Unwieldy</t>
+        </is>
+      </c>
+      <c r="U482" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -31511,6 +34111,21 @@
           <t>Type: Aura Special Rules. Armies: Elven Jesters</t>
         </is>
       </c>
+      <c r="S483" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T483" t="inlineStr">
+        <is>
+          <t>Slayer</t>
+        </is>
+      </c>
+      <c r="U483" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="484" ht="40" customHeight="1">
       <c r="A484" s="4" t="inlineStr">
@@ -31615,6 +34230,21 @@
           <t>Type: Aura Special Rules. Armies: Change Disciples, Havoc Brothers, Lust Disciples, Plague Disciples, War Disciples</t>
         </is>
       </c>
+      <c r="S485" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T485" t="inlineStr">
+        <is>
+          <t>Versatile Defense</t>
+        </is>
+      </c>
+      <c r="U485" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="486" ht="40" customHeight="1">
       <c r="A486" s="4" t="inlineStr">
@@ -31667,6 +34297,21 @@
           <t>Type: Aura Special Rules. Armies: Battle Brothers, Blood Brothers, Blood Prime Brothers, Dark Brothers, Dark Prime Brothers (+7 more)</t>
         </is>
       </c>
+      <c r="S486" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T486" t="inlineStr">
+        <is>
+          <t>Versatile Reach</t>
+        </is>
+      </c>
+      <c r="U486" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="487" ht="40" customHeight="1">
       <c r="A487" s="4" t="inlineStr">
@@ -31727,6 +34372,21 @@
           <t>Type: Aura Special Rules. Armies: Infected Colonies</t>
         </is>
       </c>
+      <c r="S487" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T487" t="inlineStr">
+        <is>
+          <t>Infected Boost</t>
+        </is>
+      </c>
+      <c r="U487" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="488" ht="40" customHeight="1">
       <c r="A488" s="4" t="inlineStr">
@@ -31855,6 +34515,21 @@
           <t>Type: Aura Special Rules. Armies: War Disciples, Wormhole Daemons of War</t>
         </is>
       </c>
+      <c r="S489" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T489" t="inlineStr">
+        <is>
+          <t>Warbound Boost</t>
+        </is>
+      </c>
+      <c r="U489" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="490" ht="40" customHeight="1">
       <c r="A490" s="4" t="inlineStr">
@@ -31965,6 +34640,21 @@
       <c r="R491" s="5" t="inlineStr">
         <is>
           <t>Type: Weapon. Armies: Wormhole Daemons of War</t>
+        </is>
+      </c>
+      <c r="S491" t="inlineStr">
+        <is>
+          <t>BOOST</t>
+        </is>
+      </c>
+      <c r="T491" t="inlineStr">
+        <is>
+          <t>Enhances Warbound</t>
+        </is>
+      </c>
+      <c r="U491" t="inlineStr">
+        <is>
+          <t>SELF</t>
         </is>
       </c>
     </row>
@@ -32019,6 +34709,21 @@
           <t>Type: Aura Special Rules. Armies: War Disciples, Wormhole Daemons of War</t>
         </is>
       </c>
+      <c r="S492" t="inlineStr">
+        <is>
+          <t>AURA</t>
+        </is>
+      </c>
+      <c r="T492" t="inlineStr">
+        <is>
+          <t>Warbound Boost</t>
+        </is>
+      </c>
+      <c r="U492" t="inlineStr">
+        <is>
+          <t>SELF_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="493" ht="40" customHeight="1">
       <c r="A493" s="4" t="inlineStr">
@@ -32079,6 +34784,21 @@
           <t>Type: Aura Special Rules. Armies: Watch Brothers, Watch Prime Brothers</t>
         </is>
       </c>
+      <c r="S493" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T493" t="inlineStr">
+        <is>
+          <t>Evasive</t>
+        </is>
+      </c>
+      <c r="U493" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="494" ht="40" customHeight="1">
       <c r="A494" s="4" t="inlineStr">
@@ -32137,6 +34857,21 @@
       <c r="R494" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Watch Brothers, Watch Prime Brothers</t>
+        </is>
+      </c>
+      <c r="S494" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T494" t="inlineStr">
+        <is>
+          <t>Unstoppable</t>
+        </is>
+      </c>
+      <c r="U494" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -32531,6 +35266,21 @@
           <t>Type: Aura Special Rules. Armies: Wolf Brothers, Wolf Prime Brothers</t>
         </is>
       </c>
+      <c r="S500" t="inlineStr">
+        <is>
+          <t>BUFF</t>
+        </is>
+      </c>
+      <c r="T500" t="inlineStr">
+        <is>
+          <t>Evasive</t>
+        </is>
+      </c>
+      <c r="U500" t="inlineStr">
+        <is>
+          <t>FRIENDLY_UNIT</t>
+        </is>
+      </c>
     </row>
     <row r="501" ht="40" customHeight="1">
       <c r="A501" s="4" t="inlineStr">
@@ -32589,6 +35339,21 @@
       <c r="R501" s="5" t="inlineStr">
         <is>
           <t>Type: Aura Special Rules. Armies: Wolf Brothers, Wolf Prime Brothers</t>
+        </is>
+      </c>
+      <c r="S501" t="inlineStr">
+        <is>
+          <t>MARK</t>
+        </is>
+      </c>
+      <c r="T501" t="inlineStr">
+        <is>
+          <t>Unstoppable</t>
+        </is>
+      </c>
+      <c r="U501" t="inlineStr">
+        <is>
+          <t>ENEMY_UNIT</t>
         </is>
       </c>
     </row>
@@ -32962,14 +35727,8 @@
           <t>COLUMN REFERENCE</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-    </row>
+    </row>
+    <row r="2"/>
     <row r="3">
       <c r="A3" s="8" t="inlineStr">
         <is>
@@ -32987,11 +35746,7 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-    </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
         <is>
@@ -33043,18 +35798,13 @@
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-    </row>
+    <row r="8"/>
     <row r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
           <t>PHASE COLUMNS</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>Mark Y if rule applies in this phase</t>
@@ -33180,19 +35930,13 @@
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-    </row>
+    <row r="17"/>
     <row r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
           <t>ENGINE CONFIGURATION</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="8" t="inlineStr">
@@ -33212,7 +35956,6 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
           <t>CALC_ATTACKS</t>
@@ -33225,7 +35968,6 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
           <t>HIT_ROLL</t>
@@ -33238,7 +35980,6 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
           <t>AFTER_HIT</t>
@@ -33251,7 +35992,6 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr">
         <is>
           <t>CALC_AP</t>
@@ -33264,7 +36004,6 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
           <t>DEF_ROLL</t>
@@ -33277,7 +36016,6 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
       <c r="B25" t="inlineStr">
         <is>
           <t>AFTER_DEF</t>
@@ -33290,7 +36028,6 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
       <c r="B26" t="inlineStr">
         <is>
           <t>AFTER_WOUND</t>
@@ -33303,7 +36040,6 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
           <t>ALLOCATE</t>
@@ -33316,7 +36052,6 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
           <t>REGEN</t>
@@ -33329,7 +36064,6 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
           <t>MORALE</t>
@@ -33342,7 +36076,6 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
           <t>ROUND_START</t>
@@ -33355,7 +36088,6 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
           <t>ROUND_END</t>
@@ -33368,7 +36100,6 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
           <t>ON_DEATH</t>
@@ -33381,7 +36112,6 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
           <t>PRE_ATTACK</t>
@@ -33394,7 +36124,6 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr">
         <is>
           <t>COMBAT_ORDER</t>
@@ -33407,7 +36136,6 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
           <t>MOVEMENT</t>
@@ -33420,7 +36148,6 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
           <t>DEPLOYMENT</t>
@@ -33433,7 +36160,6 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
       <c r="B37" t="inlineStr">
         <is>
           <t>DIRECT_DAMAGE</t>
@@ -33445,11 +36171,7 @@
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr"/>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-    </row>
+    <row r="38"/>
     <row r="39">
       <c r="A39" s="8" t="inlineStr">
         <is>
@@ -33468,7 +36190,6 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
           <t>always</t>
@@ -33481,7 +36202,6 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
           <t>is_charging</t>
@@ -33494,7 +36214,6 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
           <t>is_charged</t>
@@ -33507,7 +36226,6 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
           <t>unmodified_6_hit</t>
@@ -33520,7 +36238,6 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
           <t>phase_is_shooting</t>
@@ -33533,7 +36250,6 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
           <t>phase_is_melee</t>
@@ -33546,7 +36262,6 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
           <t>range_over_9</t>
@@ -33559,7 +36274,6 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
           <t>range_over_12</t>
@@ -33572,7 +36286,6 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
           <t>attack_not_spell</t>
@@ -33585,7 +36298,6 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
           <t>once_per_game</t>
@@ -33598,7 +36310,6 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
           <t>once_per_activation</t>
@@ -33610,11 +36321,7 @@
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr"/>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-    </row>
+    <row r="51"/>
     <row r="52">
       <c r="A52" s="8" t="inlineStr">
         <is>
@@ -33633,7 +36340,6 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr"/>
       <c r="B53" t="inlineStr">
         <is>
           <t>ADD</t>
@@ -33646,7 +36352,6 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr"/>
       <c r="B54" t="inlineStr">
         <is>
           <t>MULTIPLY</t>
@@ -33659,7 +36364,6 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
           <t>SET</t>
@@ -33672,7 +36376,6 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
           <t>REROLL</t>
@@ -33685,7 +36388,6 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
           <t>REPLACE</t>
@@ -33698,7 +36400,6 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr"/>
       <c r="B58" t="inlineStr">
         <is>
           <t>NEGATE</t>
@@ -33711,7 +36412,6 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr">
         <is>
           <t>ROLL</t>
@@ -33724,7 +36424,6 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr"/>
       <c r="B60" t="inlineStr">
         <is>
           <t>CHOOSE</t>
@@ -33737,7 +36436,6 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr"/>
       <c r="B61" t="inlineStr">
         <is>
           <t>TRIGGER</t>
@@ -33750,7 +36448,6 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr"/>
       <c r="B62" t="inlineStr">
         <is>
           <t>ENABLE</t>
@@ -33763,7 +36460,6 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr">
         <is>
           <t>GRANT</t>
@@ -33776,7 +36472,6 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr"/>
       <c r="B64" t="inlineStr">
         <is>
           <t>DAMAGE</t>
@@ -33788,11 +36483,7 @@
         </is>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr"/>
-      <c r="B65" t="inlineStr"/>
-      <c r="C65" t="inlineStr"/>
-    </row>
+    <row r="65"/>
     <row r="66">
       <c r="A66" s="8" t="inlineStr">
         <is>
@@ -33811,7 +36502,6 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr">
         <is>
           <t>attacks</t>
@@ -33824,7 +36514,6 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr"/>
       <c r="B68" t="inlineStr">
         <is>
           <t>hits</t>
@@ -33837,7 +36526,6 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr"/>
       <c r="B69" t="inlineStr">
         <is>
           <t>quality_mod</t>
@@ -33850,7 +36538,6 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr"/>
       <c r="B70" t="inlineStr">
         <is>
           <t>ap</t>
@@ -33863,7 +36550,6 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr">
         <is>
           <t>defense_target</t>
@@ -33876,7 +36562,6 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
       <c r="B72" t="inlineStr">
         <is>
           <t>defense_mod</t>
@@ -33889,7 +36574,6 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr"/>
       <c r="B73" t="inlineStr">
         <is>
           <t>wounds</t>
@@ -33902,7 +36586,6 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr"/>
       <c r="B74" t="inlineStr">
         <is>
           <t>regeneration</t>
@@ -33915,7 +36598,6 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr"/>
       <c r="B75" t="inlineStr">
         <is>
           <t>morale_mod</t>
@@ -33928,7 +36610,6 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr"/>
       <c r="B76" t="inlineStr">
         <is>
           <t>direct_hits</t>
@@ -33940,11 +36621,7 @@
         </is>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="inlineStr"/>
-      <c r="B77" t="inlineStr"/>
-      <c r="C77" t="inlineStr"/>
-    </row>
+    <row r="77"/>
     <row r="78">
       <c r="A78" s="8" t="inlineStr">
         <is>
@@ -33963,7 +36640,6 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr">
         <is>
           <t>SELF</t>
@@ -33976,7 +36652,6 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr"/>
       <c r="B80" t="inlineStr">
         <is>
           <t>ENEMY</t>
@@ -33989,7 +36664,6 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr"/>
       <c r="B81" t="inlineStr">
         <is>
           <t>WEAPON</t>
@@ -34002,7 +36676,6 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr"/>
       <c r="B82" t="inlineStr">
         <is>
           <t>FRIENDLY</t>
@@ -34014,11 +36687,7 @@
         </is>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="inlineStr"/>
-      <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
-    </row>
+    <row r="83"/>
     <row r="84">
       <c r="A84" s="8" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fix 104 direct damage rules to use DEAL_HITS effect type
Rules like Art of Pain, Flame Bots, etc. that deal direct hits
were incorrectly marked with SET, MULTIPLY, or GRANT effect types.
Updated all "takes X hits" rules to:
- Effect Type: DEAL_HITS
- Effect Target: enemy_unit
- Effect Value: X hits, [modifiers like AP(2), Deadly(3)]

These are NOT granting rules - they deal damage directly.
</commit_message>
<xml_diff>
--- a/docs/special_rules_review_matrix.xlsx
+++ b/docs/special_rules_review_matrix.xlsx
@@ -5318,17 +5318,17 @@
       </c>
       <c r="M68" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N68" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O68" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with AP (2) and Deadly (3)</t>
         </is>
       </c>
       <c r="P68" s="4" t="inlineStr">
@@ -6165,17 +6165,17 @@
       </c>
       <c r="M80" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N80" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O80" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Shatter</t>
         </is>
       </c>
       <c r="P80" s="4" t="inlineStr">
@@ -6308,17 +6308,17 @@
       </c>
       <c r="M82" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N82" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O82" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Surge</t>
         </is>
       </c>
       <c r="P82" s="4" t="inlineStr">
@@ -6376,17 +6376,17 @@
       </c>
       <c r="M83" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N83" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O83" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1 hits, with AP (2) and Deadly (3)</t>
         </is>
       </c>
       <c r="P83" s="4" t="inlineStr">
@@ -6894,17 +6894,17 @@
       </c>
       <c r="M90" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N90" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O90" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits, with Smash</t>
         </is>
       </c>
       <c r="P90" s="4" t="inlineStr">
@@ -6962,17 +6962,17 @@
       </c>
       <c r="M91" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N91" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O91" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Demolish</t>
         </is>
       </c>
       <c r="P91" s="4" t="inlineStr">
@@ -7102,17 +7102,17 @@
       </c>
       <c r="M93" s="4" t="inlineStr">
         <is>
-          <t>MULTIPLY</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N93" s="7" t="inlineStr">
         <is>
-          <t>hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O93" s="7" t="inlineStr">
         <is>
-          <t>min(3, enemy_models)</t>
+          <t>2 hits, with Blast (3)</t>
         </is>
       </c>
       <c r="P93" s="4" t="inlineStr">
@@ -7305,17 +7305,17 @@
       </c>
       <c r="M96" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N96" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O96" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3 hits, with AP (2) and Deadly (3)</t>
         </is>
       </c>
       <c r="P96" s="4" t="inlineStr">
@@ -7513,17 +7513,17 @@
       </c>
       <c r="M99" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N99" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O99" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1 hits, with AP (4)</t>
         </is>
       </c>
       <c r="P99" s="4" t="inlineStr">
@@ -7581,17 +7581,17 @@
       </c>
       <c r="M100" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N100" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O100" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits, with Blast (3) and AP (1)</t>
         </is>
       </c>
       <c r="P100" s="4" t="inlineStr">
@@ -7792,17 +7792,17 @@
       </c>
       <c r="M103" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N103" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O103" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits, with Break</t>
         </is>
       </c>
       <c r="P103" s="4" t="inlineStr">
@@ -8427,17 +8427,17 @@
       </c>
       <c r="M112" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N112" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O112" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits, with Smash</t>
         </is>
       </c>
       <c r="P112" s="4" t="inlineStr">
@@ -8931,17 +8931,17 @@
       </c>
       <c r="M119" s="4" t="inlineStr">
         <is>
-          <t>MULTIPLY</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N119" s="7" t="inlineStr">
         <is>
-          <t>hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O119" s="7" t="inlineStr">
         <is>
-          <t>min(3, enemy_models)</t>
+          <t>3 hits, with Blast (3)</t>
         </is>
       </c>
       <c r="P119" s="4" t="inlineStr">
@@ -9608,17 +9608,17 @@
       </c>
       <c r="M129" s="4" t="inlineStr">
         <is>
-          <t>MULTIPLY</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N129" s="7" t="inlineStr">
         <is>
-          <t>hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O129" s="7" t="inlineStr">
         <is>
-          <t>min(3, enemy_models)</t>
+          <t>3 hits, with Blast (3)</t>
         </is>
       </c>
       <c r="P129" s="4" t="inlineStr">
@@ -9755,17 +9755,17 @@
       </c>
       <c r="M131" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N131" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O131" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits</t>
         </is>
       </c>
       <c r="P131" s="4" t="inlineStr">
@@ -9827,17 +9827,17 @@
       </c>
       <c r="M132" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N132" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O132" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P132" s="4" t="inlineStr">
@@ -9899,17 +9899,17 @@
       </c>
       <c r="M133" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N133" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O133" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P133" s="4" t="inlineStr">
@@ -10035,17 +10035,17 @@
       </c>
       <c r="M135" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N135" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O135" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6 hits, with AP (2)</t>
         </is>
       </c>
       <c r="P135" s="4" t="inlineStr">
@@ -10523,17 +10523,17 @@
       </c>
       <c r="M142" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N142" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O142" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits, with Smash</t>
         </is>
       </c>
       <c r="P142" s="4" t="inlineStr">
@@ -10591,17 +10591,17 @@
       </c>
       <c r="M143" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N143" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O143" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Demolish</t>
         </is>
       </c>
       <c r="P143" s="4" t="inlineStr">
@@ -10735,17 +10735,17 @@
       </c>
       <c r="M145" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N145" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O145" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits, with Bane</t>
         </is>
       </c>
       <c r="P145" s="4" t="inlineStr">
@@ -10803,17 +10803,17 @@
       </c>
       <c r="M146" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N146" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O146" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1 hits, with AP (2) and Impale</t>
         </is>
       </c>
       <c r="P146" s="4" t="inlineStr">
@@ -11666,17 +11666,17 @@
       </c>
       <c r="M159" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N159" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O159" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits, with Decimate</t>
         </is>
       </c>
       <c r="P159" s="4" t="inlineStr">
@@ -12004,17 +12004,17 @@
       </c>
       <c r="M164" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N164" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O164" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with AP (2) and Deadly (3)</t>
         </is>
       </c>
       <c r="P164" s="4" t="inlineStr">
@@ -12072,17 +12072,17 @@
       </c>
       <c r="M165" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N165" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O165" s="7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>9 hits</t>
         </is>
       </c>
       <c r="P165" s="4" t="inlineStr">
@@ -12140,17 +12140,17 @@
       </c>
       <c r="M166" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N166" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O166" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Tear</t>
         </is>
       </c>
       <c r="P166" s="4" t="inlineStr">
@@ -12283,17 +12283,17 @@
       </c>
       <c r="M168" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N168" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O168" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Fracture</t>
         </is>
       </c>
       <c r="P168" s="4" t="inlineStr">
@@ -12351,17 +12351,17 @@
       </c>
       <c r="M169" s="4" t="inlineStr">
         <is>
-          <t>MULTIPLY</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N169" s="7" t="inlineStr">
         <is>
-          <t>hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O169" s="7" t="inlineStr">
         <is>
-          <t>min(3, enemy_models)</t>
+          <t>1 hits, with Blast (3)</t>
         </is>
       </c>
       <c r="P169" s="4" t="inlineStr">
@@ -12569,17 +12569,17 @@
       </c>
       <c r="M172" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N172" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O172" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits, with Purge</t>
         </is>
       </c>
       <c r="P172" s="4" t="inlineStr">
@@ -12836,17 +12836,17 @@
       </c>
       <c r="M176" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N176" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O176" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P176" s="4" t="inlineStr">
@@ -13155,17 +13155,17 @@
       </c>
       <c r="M181" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N181" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O181" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits</t>
         </is>
       </c>
       <c r="P181" s="4" t="inlineStr">
@@ -13445,17 +13445,17 @@
       </c>
       <c r="M185" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N185" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O185" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3 hits, with AP (2) and Deadly (3)</t>
         </is>
       </c>
       <c r="P185" s="4" t="inlineStr">
@@ -13798,11 +13798,19 @@
       </c>
       <c r="M190" s="4" t="inlineStr">
         <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="N190" s="7" t="inlineStr"/>
-      <c r="O190" s="7" t="inlineStr"/>
+          <t>DEAL_HITS</t>
+        </is>
+      </c>
+      <c r="N190" s="7" t="inlineStr">
+        <is>
+          <t>enemy_unit</t>
+        </is>
+      </c>
+      <c r="O190" s="7" t="inlineStr">
+        <is>
+          <t>4 hits, each</t>
+        </is>
+      </c>
       <c r="P190" s="4" t="inlineStr">
         <is>
           <t>ENEMY</t>
@@ -13858,17 +13866,17 @@
       </c>
       <c r="M191" s="4" t="inlineStr">
         <is>
-          <t>MULTIPLY</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N191" s="7" t="inlineStr">
         <is>
-          <t>hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O191" s="7" t="inlineStr">
         <is>
-          <t>min(3, enemy_models)</t>
+          <t>1 hits, with Blast (3)</t>
         </is>
       </c>
       <c r="P191" s="4" t="inlineStr">
@@ -14001,17 +14009,17 @@
       </c>
       <c r="M193" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N193" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O193" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Shred</t>
         </is>
       </c>
       <c r="P193" s="4" t="inlineStr">
@@ -14586,17 +14594,17 @@
       </c>
       <c r="M201" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N201" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O201" s="7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>9 hits, with Destructive</t>
         </is>
       </c>
       <c r="P201" s="4" t="inlineStr">
@@ -14654,17 +14662,17 @@
       </c>
       <c r="M202" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N202" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O202" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2 hits, with AP (4)</t>
         </is>
       </c>
       <c r="P202" s="4" t="inlineStr">
@@ -15629,17 +15637,17 @@
       </c>
       <c r="M216" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N216" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O216" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1) and Slam</t>
         </is>
       </c>
       <c r="P216" s="4" t="inlineStr">
@@ -15697,11 +15705,19 @@
       </c>
       <c r="M217" s="4" t="inlineStr">
         <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="N217" s="7" t="inlineStr"/>
-      <c r="O217" s="7" t="inlineStr"/>
+          <t>DEAL_HITS</t>
+        </is>
+      </c>
+      <c r="N217" s="7" t="inlineStr">
+        <is>
+          <t>enemy_unit</t>
+        </is>
+      </c>
+      <c r="O217" s="7" t="inlineStr">
+        <is>
+          <t>4 hits, each</t>
+        </is>
+      </c>
       <c r="P217" s="4" t="inlineStr">
         <is>
           <t>ENEMY</t>
@@ -15757,17 +15773,17 @@
       </c>
       <c r="M218" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N218" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O218" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with AP (2)</t>
         </is>
       </c>
       <c r="P218" s="4" t="inlineStr">
@@ -16111,17 +16127,17 @@
       </c>
       <c r="M223" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N223" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O223" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3 hits, with AP (2) each</t>
         </is>
       </c>
       <c r="P223" s="4" t="inlineStr">
@@ -16179,17 +16195,17 @@
       </c>
       <c r="M224" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N224" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O224" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P224" s="4" t="inlineStr">
@@ -16918,17 +16934,17 @@
       </c>
       <c r="M235" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N235" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O235" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P235" s="4" t="inlineStr">
@@ -17121,17 +17137,17 @@
       </c>
       <c r="M238" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N238" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O238" s="7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>9 hits</t>
         </is>
       </c>
       <c r="P238" s="4" t="inlineStr">
@@ -18571,17 +18587,17 @@
       </c>
       <c r="M259" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N259" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O259" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1) and Shred</t>
         </is>
       </c>
       <c r="P259" s="4" t="inlineStr">
@@ -18639,17 +18655,17 @@
       </c>
       <c r="M260" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N260" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O260" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P260" s="4" t="inlineStr">
@@ -18857,17 +18873,17 @@
       </c>
       <c r="M263" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N263" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O263" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits, with Smash</t>
         </is>
       </c>
       <c r="P263" s="4" t="inlineStr">
@@ -18925,17 +18941,17 @@
       </c>
       <c r="M264" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N264" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O264" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Demolish</t>
         </is>
       </c>
       <c r="P264" s="4" t="inlineStr">
@@ -19121,17 +19137,17 @@
       </c>
       <c r="M267" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N267" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O267" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4 hits, with AP (1) and Fragment</t>
         </is>
       </c>
       <c r="P267" s="4" t="inlineStr">
@@ -19189,11 +19205,19 @@
       </c>
       <c r="M268" s="4" t="inlineStr">
         <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="N268" s="7" t="inlineStr"/>
-      <c r="O268" s="7" t="inlineStr"/>
+          <t>DEAL_HITS</t>
+        </is>
+      </c>
+      <c r="N268" s="7" t="inlineStr">
+        <is>
+          <t>enemy_unit</t>
+        </is>
+      </c>
+      <c r="O268" s="7" t="inlineStr">
+        <is>
+          <t>4 hits, each</t>
+        </is>
+      </c>
       <c r="P268" s="4" t="inlineStr">
         <is>
           <t>ENEMY</t>
@@ -20220,17 +20244,17 @@
       </c>
       <c r="M283" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N283" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O283" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Surge</t>
         </is>
       </c>
       <c r="P283" s="4" t="inlineStr">
@@ -20356,17 +20380,17 @@
       </c>
       <c r="M285" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N285" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O285" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Surge</t>
         </is>
       </c>
       <c r="P285" s="4" t="inlineStr">
@@ -20424,17 +20448,17 @@
       </c>
       <c r="M286" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N286" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O286" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1) and Shred</t>
         </is>
       </c>
       <c r="P286" s="4" t="inlineStr">
@@ -20552,17 +20576,17 @@
       </c>
       <c r="M288" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N288" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O288" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with AP (2) each</t>
         </is>
       </c>
       <c r="P288" s="4" t="inlineStr">
@@ -20620,17 +20644,17 @@
       </c>
       <c r="M289" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N289" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O289" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Demolish</t>
         </is>
       </c>
       <c r="P289" s="4" t="inlineStr">
@@ -21034,11 +21058,19 @@
       </c>
       <c r="M295" s="4" t="inlineStr">
         <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="N295" s="7" t="inlineStr"/>
-      <c r="O295" s="7" t="inlineStr"/>
+          <t>DEAL_HITS</t>
+        </is>
+      </c>
+      <c r="N295" s="7" t="inlineStr">
+        <is>
+          <t>enemy_unit</t>
+        </is>
+      </c>
+      <c r="O295" s="7" t="inlineStr">
+        <is>
+          <t>4 hits, each</t>
+        </is>
+      </c>
       <c r="P295" s="4" t="inlineStr">
         <is>
           <t>ENEMY</t>
@@ -21236,17 +21268,17 @@
       </c>
       <c r="M298" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N298" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O298" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1) and Shred</t>
         </is>
       </c>
       <c r="P298" s="4" t="inlineStr">
@@ -21304,17 +21336,17 @@
       </c>
       <c r="M299" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N299" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O299" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Rupture</t>
         </is>
       </c>
       <c r="P299" s="4" t="inlineStr">
@@ -21514,17 +21546,17 @@
       </c>
       <c r="M302" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N302" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O302" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with AP (2)</t>
         </is>
       </c>
       <c r="P302" s="4" t="inlineStr">
@@ -21803,17 +21835,17 @@
       </c>
       <c r="M306" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N306" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O306" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3 hits, with AP (4)</t>
         </is>
       </c>
       <c r="P306" s="4" t="inlineStr">
@@ -22293,11 +22325,19 @@
       </c>
       <c r="M313" s="4" t="inlineStr">
         <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="N313" s="7" t="inlineStr"/>
-      <c r="O313" s="7" t="inlineStr"/>
+          <t>DEAL_HITS</t>
+        </is>
+      </c>
+      <c r="N313" s="7" t="inlineStr">
+        <is>
+          <t>enemy_unit</t>
+        </is>
+      </c>
+      <c r="O313" s="7" t="inlineStr">
+        <is>
+          <t>4 hits, each</t>
+        </is>
+      </c>
       <c r="P313" s="4" t="inlineStr">
         <is>
           <t>ENEMY</t>
@@ -22428,17 +22468,17 @@
       </c>
       <c r="M315" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N315" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O315" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2 hits, with AP (4)</t>
         </is>
       </c>
       <c r="P315" s="4" t="inlineStr">
@@ -22789,17 +22829,17 @@
       </c>
       <c r="M320" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N320" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O320" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3 hits, with AP (2) and Skewer</t>
         </is>
       </c>
       <c r="P320" s="4" t="inlineStr">
@@ -22857,17 +22897,17 @@
       </c>
       <c r="M321" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N321" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O321" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P321" s="4" t="inlineStr">
@@ -22925,17 +22965,17 @@
       </c>
       <c r="M322" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N322" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O322" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6 hits, with AP (2)</t>
         </is>
       </c>
       <c r="P322" s="4" t="inlineStr">
@@ -23068,17 +23108,17 @@
       </c>
       <c r="M324" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N324" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O324" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1 hits, with AP (2) each</t>
         </is>
       </c>
       <c r="P324" s="4" t="inlineStr">
@@ -23136,17 +23176,17 @@
       </c>
       <c r="M325" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N325" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O325" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits, with Hazardous</t>
         </is>
       </c>
       <c r="P325" s="4" t="inlineStr">
@@ -24510,17 +24550,17 @@
       </c>
       <c r="M344" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N344" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O344" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2 hits, with AP (4)</t>
         </is>
       </c>
       <c r="P344" s="4" t="inlineStr">
@@ -24728,17 +24768,17 @@
       </c>
       <c r="M347" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N347" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O347" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4 hits, with AP (2)</t>
         </is>
       </c>
       <c r="P347" s="4" t="inlineStr">
@@ -24796,17 +24836,17 @@
       </c>
       <c r="M348" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N348" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O348" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 hits, with Reap</t>
         </is>
       </c>
       <c r="P348" s="4" t="inlineStr">
@@ -24939,17 +24979,17 @@
       </c>
       <c r="M350" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N350" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O350" s="7" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>9 hits, with Bane</t>
         </is>
       </c>
       <c r="P350" s="4" t="inlineStr">
@@ -25007,17 +25047,17 @@
       </c>
       <c r="M351" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N351" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O351" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits, with Bane</t>
         </is>
       </c>
       <c r="P351" s="4" t="inlineStr">
@@ -25147,17 +25187,17 @@
       </c>
       <c r="M353" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N353" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O353" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3 hits, with AP (2) each</t>
         </is>
       </c>
       <c r="P353" s="4" t="inlineStr">
@@ -25533,17 +25573,17 @@
       </c>
       <c r="M359" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N359" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O359" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4 hits, with Scratch</t>
         </is>
       </c>
       <c r="P359" s="4" t="inlineStr">
@@ -26291,17 +26331,17 @@
       </c>
       <c r="M370" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N370" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O370" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Butcher</t>
         </is>
       </c>
       <c r="P370" s="4" t="inlineStr">
@@ -27728,17 +27768,17 @@
       </c>
       <c r="M391" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N391" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O391" s="7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1 hits, with AP (4)</t>
         </is>
       </c>
       <c r="P391" s="4" t="inlineStr">
@@ -27796,17 +27836,17 @@
       </c>
       <c r="M392" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N392" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O392" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits</t>
         </is>
       </c>
       <c r="P392" s="4" t="inlineStr">
@@ -28349,17 +28389,17 @@
       </c>
       <c r="M400" s="4" t="inlineStr">
         <is>
-          <t>MULTIPLY</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N400" s="7" t="inlineStr">
         <is>
-          <t>hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O400" s="7" t="inlineStr">
         <is>
-          <t>min(3, enemy_models)</t>
+          <t>3 hits, with Blast (3)</t>
         </is>
       </c>
       <c r="P400" s="4" t="inlineStr">
@@ -28417,17 +28457,17 @@
       </c>
       <c r="M401" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N401" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O401" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits</t>
         </is>
       </c>
       <c r="P401" s="4" t="inlineStr">
@@ -28485,17 +28525,17 @@
       </c>
       <c r="M402" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N402" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O402" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4 hits, with AP (1) and Wreck</t>
         </is>
       </c>
       <c r="P402" s="4" t="inlineStr">
@@ -28760,17 +28800,17 @@
       </c>
       <c r="M406" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N406" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O406" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Disintegrate</t>
         </is>
       </c>
       <c r="P406" s="4" t="inlineStr">
@@ -28975,17 +29015,17 @@
       </c>
       <c r="M409" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N409" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O409" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1) and Crack</t>
         </is>
       </c>
       <c r="P409" s="4" t="inlineStr">
@@ -29043,17 +29083,17 @@
       </c>
       <c r="M410" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N410" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O410" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1) and Shred</t>
         </is>
       </c>
       <c r="P410" s="4" t="inlineStr">
@@ -29761,17 +29801,17 @@
       </c>
       <c r="M420" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N420" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O420" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Slash</t>
         </is>
       </c>
       <c r="P420" s="4" t="inlineStr">
@@ -30040,17 +30080,17 @@
       </c>
       <c r="M424" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N424" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O424" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4 hits, with AP (1) and Quake</t>
         </is>
       </c>
       <c r="P424" s="4" t="inlineStr">
@@ -30108,17 +30148,17 @@
       </c>
       <c r="M425" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N425" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O425" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Lacerate</t>
         </is>
       </c>
       <c r="P425" s="4" t="inlineStr">
@@ -30176,17 +30216,17 @@
       </c>
       <c r="M426" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N426" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O426" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits, with Puncture</t>
         </is>
       </c>
       <c r="P426" s="4" t="inlineStr">
@@ -30825,17 +30865,17 @@
       </c>
       <c r="M436" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N436" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O436" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Bash</t>
         </is>
       </c>
       <c r="P436" s="4" t="inlineStr">
@@ -31241,17 +31281,17 @@
       </c>
       <c r="M442" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N442" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O442" s="7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3 hits, with Shred</t>
         </is>
       </c>
       <c r="P442" s="4" t="inlineStr">
@@ -31313,17 +31353,17 @@
       </c>
       <c r="M443" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N443" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O443" s="7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3 hits, with Surge (roll one die per hit to see if it triggers)</t>
         </is>
       </c>
       <c r="P443" s="4" t="inlineStr">
@@ -31385,17 +31425,17 @@
       </c>
       <c r="M444" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N444" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O444" s="7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3 hits, with Bane</t>
         </is>
       </c>
       <c r="P444" s="4" t="inlineStr">
@@ -31453,17 +31493,17 @@
       </c>
       <c r="M445" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N445" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O445" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6 hits, with AP (1) and Surge</t>
         </is>
       </c>
       <c r="P445" s="4" t="inlineStr">
@@ -31525,17 +31565,17 @@
       </c>
       <c r="M446" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N446" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O446" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P446" s="4" t="inlineStr">
@@ -31879,17 +31919,17 @@
       </c>
       <c r="M451" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N451" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O451" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P451" s="4" t="inlineStr">
@@ -32217,17 +32257,17 @@
       </c>
       <c r="M456" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N456" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O456" s="7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6 hits</t>
         </is>
       </c>
       <c r="P456" s="4" t="inlineStr">
@@ -33092,17 +33132,17 @@
       </c>
       <c r="M469" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N469" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O469" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits</t>
         </is>
       </c>
       <c r="P469" s="4" t="inlineStr">
@@ -33160,17 +33200,17 @@
       </c>
       <c r="M470" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N470" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O470" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4 hits, with AP (1)</t>
         </is>
       </c>
       <c r="P470" s="4" t="inlineStr">
@@ -34427,17 +34467,17 @@
       </c>
       <c r="M488" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N488" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O488" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3 hits, with AP (2) and Deadly (3)</t>
         </is>
       </c>
       <c r="P488" s="4" t="inlineStr">
@@ -34914,17 +34954,17 @@
       </c>
       <c r="M495" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N495" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O495" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits, with Smash</t>
         </is>
       </c>
       <c r="P495" s="4" t="inlineStr">
@@ -34982,17 +35022,17 @@
       </c>
       <c r="M496" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N496" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O496" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Demolish</t>
         </is>
       </c>
       <c r="P496" s="4" t="inlineStr">
@@ -35118,17 +35158,17 @@
       </c>
       <c r="M498" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N498" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O498" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Thrash</t>
         </is>
       </c>
       <c r="P498" s="4" t="inlineStr">
@@ -35396,17 +35436,17 @@
       </c>
       <c r="M502" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N502" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O502" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1 hits, with Smash</t>
         </is>
       </c>
       <c r="P502" s="4" t="inlineStr">
@@ -35464,17 +35504,17 @@
       </c>
       <c r="M503" s="4" t="inlineStr">
         <is>
-          <t>DAMAGE</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N503" s="7" t="inlineStr">
         <is>
-          <t>direct_hits</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O503" s="7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 hits, with Demolish</t>
         </is>
       </c>
       <c r="P503" s="4" t="inlineStr">
@@ -35660,17 +35700,17 @@
       </c>
       <c r="M506" s="4" t="inlineStr">
         <is>
-          <t>SET</t>
+          <t>DEAL_HITS</t>
         </is>
       </c>
       <c r="N506" s="7" t="inlineStr">
         <is>
-          <t>ap</t>
+          <t>enemy_unit</t>
         </is>
       </c>
       <c r="O506" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2 hits, with AP (1) and Surge</t>
         </is>
       </c>
       <c r="P506" s="4" t="inlineStr">
@@ -35728,7 +35768,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="8" t="inlineStr">
         <is>
@@ -35746,7 +35785,6 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
         <is>
@@ -35798,7 +35836,6 @@
         </is>
       </c>
     </row>
-    <row r="8"/>
     <row r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
@@ -35930,7 +35967,6 @@
         </is>
       </c>
     </row>
-    <row r="17"/>
     <row r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
@@ -36171,7 +36207,6 @@
         </is>
       </c>
     </row>
-    <row r="38"/>
     <row r="39">
       <c r="A39" s="8" t="inlineStr">
         <is>
@@ -36321,7 +36356,6 @@
         </is>
       </c>
     </row>
-    <row r="51"/>
     <row r="52">
       <c r="A52" s="8" t="inlineStr">
         <is>
@@ -36483,7 +36517,6 @@
         </is>
       </c>
     </row>
-    <row r="65"/>
     <row r="66">
       <c r="A66" s="8" t="inlineStr">
         <is>
@@ -36621,7 +36654,6 @@
         </is>
       </c>
     </row>
-    <row r="77"/>
     <row r="78">
       <c r="A78" s="8" t="inlineStr">
         <is>
@@ -36687,7 +36719,6 @@
         </is>
       </c>
     </row>
-    <row r="83"/>
     <row r="84">
       <c r="A84" s="8" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fix DEAL_HITS rules trigger timing
Direct damage rules like Art of Pain trigger at the start of unit
activation, not at round start/end. Updated 104 rules:
- Cleared RND column (was incorrectly marked as round phase)
- Set Trigger Step to ACTIVATION_START
- Set Trigger Condition to once_per_activation or once_per_game
</commit_message>
<xml_diff>
--- a/docs/special_rules_review_matrix.xlsx
+++ b/docs/special_rules_review_matrix.xlsx
@@ -5301,19 +5301,15 @@
       <c r="G68" s="4" t="inlineStr"/>
       <c r="H68" s="4" t="inlineStr"/>
       <c r="I68" s="4" t="inlineStr"/>
-      <c r="J68" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J68" s="6" t="n"/>
       <c r="K68" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L68" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M68" s="4" t="inlineStr">
@@ -6148,19 +6144,15 @@
       <c r="G80" s="4" t="inlineStr"/>
       <c r="H80" s="4" t="inlineStr"/>
       <c r="I80" s="4" t="inlineStr"/>
-      <c r="J80" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J80" s="6" t="n"/>
       <c r="K80" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L80" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M80" s="4" t="inlineStr">
@@ -6291,19 +6283,15 @@
       <c r="G82" s="4" t="inlineStr"/>
       <c r="H82" s="4" t="inlineStr"/>
       <c r="I82" s="4" t="inlineStr"/>
-      <c r="J82" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J82" s="6" t="n"/>
       <c r="K82" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L82" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M82" s="4" t="inlineStr">
@@ -6359,19 +6347,15 @@
       <c r="G83" s="4" t="inlineStr"/>
       <c r="H83" s="4" t="inlineStr"/>
       <c r="I83" s="4" t="inlineStr"/>
-      <c r="J83" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J83" s="6" t="n"/>
       <c r="K83" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L83" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M83" s="4" t="inlineStr">
@@ -6877,19 +6861,15 @@
       <c r="G90" s="4" t="inlineStr"/>
       <c r="H90" s="4" t="inlineStr"/>
       <c r="I90" s="4" t="inlineStr"/>
-      <c r="J90" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J90" s="6" t="n"/>
       <c r="K90" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L90" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M90" s="4" t="inlineStr">
@@ -6945,19 +6925,15 @@
       <c r="G91" s="4" t="inlineStr"/>
       <c r="H91" s="4" t="inlineStr"/>
       <c r="I91" s="4" t="inlineStr"/>
-      <c r="J91" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J91" s="6" t="n"/>
       <c r="K91" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L91" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M91" s="4" t="inlineStr">
@@ -7085,19 +7061,15 @@
       <c r="G93" s="4" t="inlineStr"/>
       <c r="H93" s="4" t="inlineStr"/>
       <c r="I93" s="4" t="inlineStr"/>
-      <c r="J93" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J93" s="6" t="n"/>
       <c r="K93" s="7" t="inlineStr">
         <is>
-          <t>AFTER_HIT</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L93" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M93" s="4" t="inlineStr">
@@ -7288,19 +7260,15 @@
       <c r="G96" s="4" t="inlineStr"/>
       <c r="H96" s="4" t="inlineStr"/>
       <c r="I96" s="4" t="inlineStr"/>
-      <c r="J96" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J96" s="6" t="n"/>
       <c r="K96" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L96" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M96" s="4" t="inlineStr">
@@ -7496,19 +7464,15 @@
       <c r="G99" s="4" t="inlineStr"/>
       <c r="H99" s="4" t="inlineStr"/>
       <c r="I99" s="4" t="inlineStr"/>
-      <c r="J99" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J99" s="6" t="n"/>
       <c r="K99" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L99" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M99" s="4" t="inlineStr">
@@ -7564,14 +7528,10 @@
       <c r="G100" s="4" t="inlineStr"/>
       <c r="H100" s="4" t="inlineStr"/>
       <c r="I100" s="4" t="inlineStr"/>
-      <c r="J100" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J100" s="6" t="n"/>
       <c r="K100" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L100" s="7" t="inlineStr">
@@ -7775,19 +7735,15 @@
       <c r="G103" s="4" t="inlineStr"/>
       <c r="H103" s="4" t="inlineStr"/>
       <c r="I103" s="4" t="inlineStr"/>
-      <c r="J103" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J103" s="6" t="n"/>
       <c r="K103" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L103" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M103" s="4" t="inlineStr">
@@ -8410,19 +8366,15 @@
       <c r="G112" s="4" t="inlineStr"/>
       <c r="H112" s="4" t="inlineStr"/>
       <c r="I112" s="4" t="inlineStr"/>
-      <c r="J112" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J112" s="6" t="n"/>
       <c r="K112" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L112" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M112" s="4" t="inlineStr">
@@ -8914,19 +8866,15 @@
       <c r="G119" s="4" t="inlineStr"/>
       <c r="H119" s="4" t="inlineStr"/>
       <c r="I119" s="4" t="inlineStr"/>
-      <c r="J119" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J119" s="6" t="n"/>
       <c r="K119" s="7" t="inlineStr">
         <is>
-          <t>AFTER_HIT</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L119" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M119" s="4" t="inlineStr">
@@ -9591,19 +9539,15 @@
       <c r="G129" s="4" t="inlineStr"/>
       <c r="H129" s="4" t="inlineStr"/>
       <c r="I129" s="4" t="inlineStr"/>
-      <c r="J129" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J129" s="6" t="n"/>
       <c r="K129" s="7" t="inlineStr">
         <is>
-          <t>AFTER_HIT</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L129" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M129" s="4" t="inlineStr">
@@ -9738,14 +9682,10 @@
       <c r="G131" s="4" t="inlineStr"/>
       <c r="H131" s="4" t="inlineStr"/>
       <c r="I131" s="4" t="inlineStr"/>
-      <c r="J131" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J131" s="6" t="n"/>
       <c r="K131" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L131" s="7" t="inlineStr">
@@ -9810,14 +9750,10 @@
       <c r="G132" s="4" t="inlineStr"/>
       <c r="H132" s="4" t="inlineStr"/>
       <c r="I132" s="4" t="inlineStr"/>
-      <c r="J132" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J132" s="6" t="n"/>
       <c r="K132" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L132" s="7" t="inlineStr">
@@ -9882,14 +9818,10 @@
       <c r="G133" s="4" t="inlineStr"/>
       <c r="H133" s="4" t="inlineStr"/>
       <c r="I133" s="4" t="inlineStr"/>
-      <c r="J133" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J133" s="6" t="n"/>
       <c r="K133" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L133" s="7" t="inlineStr">
@@ -10018,19 +9950,15 @@
       <c r="G135" s="4" t="inlineStr"/>
       <c r="H135" s="4" t="inlineStr"/>
       <c r="I135" s="4" t="inlineStr"/>
-      <c r="J135" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J135" s="6" t="n"/>
       <c r="K135" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L135" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M135" s="4" t="inlineStr">
@@ -10506,19 +10434,15 @@
       <c r="G142" s="4" t="inlineStr"/>
       <c r="H142" s="4" t="inlineStr"/>
       <c r="I142" s="4" t="inlineStr"/>
-      <c r="J142" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J142" s="6" t="n"/>
       <c r="K142" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L142" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M142" s="4" t="inlineStr">
@@ -10574,19 +10498,15 @@
       <c r="G143" s="4" t="inlineStr"/>
       <c r="H143" s="4" t="inlineStr"/>
       <c r="I143" s="4" t="inlineStr"/>
-      <c r="J143" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J143" s="6" t="n"/>
       <c r="K143" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L143" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M143" s="4" t="inlineStr">
@@ -10718,19 +10638,15 @@
       <c r="G145" s="4" t="inlineStr"/>
       <c r="H145" s="4" t="inlineStr"/>
       <c r="I145" s="4" t="inlineStr"/>
-      <c r="J145" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J145" s="6" t="n"/>
       <c r="K145" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L145" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M145" s="4" t="inlineStr">
@@ -10786,19 +10702,15 @@
       <c r="G146" s="4" t="inlineStr"/>
       <c r="H146" s="4" t="inlineStr"/>
       <c r="I146" s="4" t="inlineStr"/>
-      <c r="J146" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J146" s="6" t="n"/>
       <c r="K146" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L146" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M146" s="4" t="inlineStr">
@@ -11649,19 +11561,15 @@
       <c r="G159" s="4" t="inlineStr"/>
       <c r="H159" s="4" t="inlineStr"/>
       <c r="I159" s="4" t="inlineStr"/>
-      <c r="J159" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J159" s="6" t="n"/>
       <c r="K159" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L159" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M159" s="4" t="inlineStr">
@@ -11987,19 +11895,15 @@
       <c r="G164" s="4" t="inlineStr"/>
       <c r="H164" s="4" t="inlineStr"/>
       <c r="I164" s="4" t="inlineStr"/>
-      <c r="J164" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J164" s="6" t="n"/>
       <c r="K164" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L164" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M164" s="4" t="inlineStr">
@@ -12055,19 +11959,15 @@
       <c r="G165" s="4" t="inlineStr"/>
       <c r="H165" s="4" t="inlineStr"/>
       <c r="I165" s="4" t="inlineStr"/>
-      <c r="J165" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J165" s="6" t="n"/>
       <c r="K165" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L165" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M165" s="4" t="inlineStr">
@@ -12123,19 +12023,15 @@
       <c r="G166" s="4" t="inlineStr"/>
       <c r="H166" s="4" t="inlineStr"/>
       <c r="I166" s="4" t="inlineStr"/>
-      <c r="J166" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J166" s="6" t="n"/>
       <c r="K166" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L166" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M166" s="4" t="inlineStr">
@@ -12266,19 +12162,15 @@
       <c r="G168" s="4" t="inlineStr"/>
       <c r="H168" s="4" t="inlineStr"/>
       <c r="I168" s="4" t="inlineStr"/>
-      <c r="J168" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J168" s="6" t="n"/>
       <c r="K168" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L168" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M168" s="4" t="inlineStr">
@@ -12334,19 +12226,15 @@
       <c r="G169" s="4" t="inlineStr"/>
       <c r="H169" s="4" t="inlineStr"/>
       <c r="I169" s="4" t="inlineStr"/>
-      <c r="J169" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J169" s="6" t="n"/>
       <c r="K169" s="7" t="inlineStr">
         <is>
-          <t>AFTER_HIT</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L169" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M169" s="4" t="inlineStr">
@@ -12552,19 +12440,15 @@
       <c r="G172" s="4" t="inlineStr"/>
       <c r="H172" s="4" t="inlineStr"/>
       <c r="I172" s="4" t="inlineStr"/>
-      <c r="J172" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J172" s="6" t="n"/>
       <c r="K172" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L172" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M172" s="4" t="inlineStr">
@@ -12819,19 +12703,15 @@
       <c r="G176" s="4" t="inlineStr"/>
       <c r="H176" s="4" t="inlineStr"/>
       <c r="I176" s="4" t="inlineStr"/>
-      <c r="J176" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J176" s="6" t="n"/>
       <c r="K176" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L176" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M176" s="4" t="inlineStr">
@@ -13138,19 +13018,15 @@
       <c r="G181" s="4" t="inlineStr"/>
       <c r="H181" s="4" t="inlineStr"/>
       <c r="I181" s="4" t="inlineStr"/>
-      <c r="J181" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J181" s="6" t="n"/>
       <c r="K181" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L181" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M181" s="4" t="inlineStr">
@@ -13428,19 +13304,15 @@
       <c r="G185" s="4" t="inlineStr"/>
       <c r="H185" s="4" t="inlineStr"/>
       <c r="I185" s="4" t="inlineStr"/>
-      <c r="J185" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J185" s="6" t="n"/>
       <c r="K185" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L185" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M185" s="4" t="inlineStr">
@@ -13781,19 +13653,15 @@
       <c r="G190" s="4" t="inlineStr"/>
       <c r="H190" s="4" t="inlineStr"/>
       <c r="I190" s="4" t="inlineStr"/>
-      <c r="J190" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J190" s="6" t="n"/>
       <c r="K190" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L190" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M190" s="4" t="inlineStr">
@@ -13849,19 +13717,15 @@
       <c r="G191" s="4" t="inlineStr"/>
       <c r="H191" s="4" t="inlineStr"/>
       <c r="I191" s="4" t="inlineStr"/>
-      <c r="J191" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J191" s="6" t="n"/>
       <c r="K191" s="7" t="inlineStr">
         <is>
-          <t>AFTER_HIT</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L191" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M191" s="4" t="inlineStr">
@@ -13992,19 +13856,15 @@
       <c r="G193" s="4" t="inlineStr"/>
       <c r="H193" s="4" t="inlineStr"/>
       <c r="I193" s="4" t="inlineStr"/>
-      <c r="J193" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J193" s="6" t="n"/>
       <c r="K193" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L193" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M193" s="4" t="inlineStr">
@@ -14577,19 +14437,15 @@
       <c r="G201" s="4" t="inlineStr"/>
       <c r="H201" s="4" t="inlineStr"/>
       <c r="I201" s="4" t="inlineStr"/>
-      <c r="J201" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J201" s="6" t="n"/>
       <c r="K201" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L201" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M201" s="4" t="inlineStr">
@@ -14645,19 +14501,15 @@
       <c r="G202" s="4" t="inlineStr"/>
       <c r="H202" s="4" t="inlineStr"/>
       <c r="I202" s="4" t="inlineStr"/>
-      <c r="J202" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J202" s="6" t="n"/>
       <c r="K202" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L202" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M202" s="4" t="inlineStr">
@@ -15620,19 +15472,15 @@
       <c r="G216" s="4" t="inlineStr"/>
       <c r="H216" s="4" t="inlineStr"/>
       <c r="I216" s="4" t="inlineStr"/>
-      <c r="J216" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J216" s="6" t="n"/>
       <c r="K216" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L216" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M216" s="4" t="inlineStr">
@@ -15688,19 +15536,15 @@
       <c r="G217" s="4" t="inlineStr"/>
       <c r="H217" s="4" t="inlineStr"/>
       <c r="I217" s="4" t="inlineStr"/>
-      <c r="J217" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J217" s="6" t="n"/>
       <c r="K217" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L217" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M217" s="4" t="inlineStr">
@@ -15756,19 +15600,15 @@
       <c r="G218" s="4" t="inlineStr"/>
       <c r="H218" s="4" t="inlineStr"/>
       <c r="I218" s="4" t="inlineStr"/>
-      <c r="J218" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J218" s="6" t="n"/>
       <c r="K218" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L218" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M218" s="4" t="inlineStr">
@@ -16110,19 +15950,15 @@
       <c r="G223" s="4" t="inlineStr"/>
       <c r="H223" s="4" t="inlineStr"/>
       <c r="I223" s="4" t="inlineStr"/>
-      <c r="J223" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J223" s="6" t="n"/>
       <c r="K223" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L223" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M223" s="4" t="inlineStr">
@@ -16178,19 +16014,15 @@
       <c r="G224" s="4" t="inlineStr"/>
       <c r="H224" s="4" t="inlineStr"/>
       <c r="I224" s="4" t="inlineStr"/>
-      <c r="J224" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J224" s="6" t="n"/>
       <c r="K224" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L224" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M224" s="4" t="inlineStr">
@@ -16917,19 +16749,15 @@
       <c r="G235" s="4" t="inlineStr"/>
       <c r="H235" s="4" t="inlineStr"/>
       <c r="I235" s="4" t="inlineStr"/>
-      <c r="J235" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J235" s="6" t="n"/>
       <c r="K235" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L235" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M235" s="4" t="inlineStr">
@@ -17120,19 +16948,15 @@
       <c r="G238" s="4" t="inlineStr"/>
       <c r="H238" s="4" t="inlineStr"/>
       <c r="I238" s="4" t="inlineStr"/>
-      <c r="J238" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J238" s="6" t="n"/>
       <c r="K238" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L238" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M238" s="4" t="inlineStr">
@@ -18570,19 +18394,15 @@
       <c r="G259" s="4" t="inlineStr"/>
       <c r="H259" s="4" t="inlineStr"/>
       <c r="I259" s="4" t="inlineStr"/>
-      <c r="J259" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J259" s="6" t="n"/>
       <c r="K259" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L259" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M259" s="4" t="inlineStr">
@@ -18638,19 +18458,15 @@
       <c r="G260" s="4" t="inlineStr"/>
       <c r="H260" s="4" t="inlineStr"/>
       <c r="I260" s="4" t="inlineStr"/>
-      <c r="J260" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J260" s="6" t="n"/>
       <c r="K260" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L260" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M260" s="4" t="inlineStr">
@@ -18856,19 +18672,15 @@
       <c r="G263" s="4" t="inlineStr"/>
       <c r="H263" s="4" t="inlineStr"/>
       <c r="I263" s="4" t="inlineStr"/>
-      <c r="J263" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J263" s="6" t="n"/>
       <c r="K263" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L263" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M263" s="4" t="inlineStr">
@@ -18924,19 +18736,15 @@
       <c r="G264" s="4" t="inlineStr"/>
       <c r="H264" s="4" t="inlineStr"/>
       <c r="I264" s="4" t="inlineStr"/>
-      <c r="J264" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J264" s="6" t="n"/>
       <c r="K264" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L264" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M264" s="4" t="inlineStr">
@@ -19120,19 +18928,15 @@
       <c r="G267" s="4" t="inlineStr"/>
       <c r="H267" s="4" t="inlineStr"/>
       <c r="I267" s="4" t="inlineStr"/>
-      <c r="J267" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J267" s="6" t="n"/>
       <c r="K267" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L267" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M267" s="4" t="inlineStr">
@@ -19188,19 +18992,15 @@
       <c r="G268" s="4" t="inlineStr"/>
       <c r="H268" s="4" t="inlineStr"/>
       <c r="I268" s="4" t="inlineStr"/>
-      <c r="J268" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J268" s="6" t="n"/>
       <c r="K268" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L268" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M268" s="4" t="inlineStr">
@@ -20227,19 +20027,15 @@
       <c r="G283" s="4" t="inlineStr"/>
       <c r="H283" s="4" t="inlineStr"/>
       <c r="I283" s="4" t="inlineStr"/>
-      <c r="J283" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J283" s="6" t="n"/>
       <c r="K283" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L283" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M283" s="4" t="inlineStr">
@@ -20363,19 +20159,15 @@
       <c r="G285" s="4" t="inlineStr"/>
       <c r="H285" s="4" t="inlineStr"/>
       <c r="I285" s="4" t="inlineStr"/>
-      <c r="J285" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J285" s="6" t="n"/>
       <c r="K285" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L285" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M285" s="4" t="inlineStr">
@@ -20431,19 +20223,15 @@
       <c r="G286" s="4" t="inlineStr"/>
       <c r="H286" s="4" t="inlineStr"/>
       <c r="I286" s="4" t="inlineStr"/>
-      <c r="J286" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J286" s="6" t="n"/>
       <c r="K286" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L286" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M286" s="4" t="inlineStr">
@@ -20559,19 +20347,15 @@
       <c r="G288" s="4" t="inlineStr"/>
       <c r="H288" s="4" t="inlineStr"/>
       <c r="I288" s="4" t="inlineStr"/>
-      <c r="J288" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J288" s="6" t="n"/>
       <c r="K288" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L288" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M288" s="4" t="inlineStr">
@@ -20627,19 +20411,15 @@
       <c r="G289" s="4" t="inlineStr"/>
       <c r="H289" s="4" t="inlineStr"/>
       <c r="I289" s="4" t="inlineStr"/>
-      <c r="J289" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J289" s="6" t="n"/>
       <c r="K289" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L289" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M289" s="4" t="inlineStr">
@@ -21041,19 +20821,15 @@
       <c r="G295" s="4" t="inlineStr"/>
       <c r="H295" s="4" t="inlineStr"/>
       <c r="I295" s="4" t="inlineStr"/>
-      <c r="J295" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J295" s="6" t="n"/>
       <c r="K295" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L295" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M295" s="4" t="inlineStr">
@@ -21251,19 +21027,15 @@
       <c r="G298" s="4" t="inlineStr"/>
       <c r="H298" s="4" t="inlineStr"/>
       <c r="I298" s="4" t="inlineStr"/>
-      <c r="J298" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J298" s="6" t="n"/>
       <c r="K298" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L298" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M298" s="4" t="inlineStr">
@@ -21319,19 +21091,15 @@
       <c r="G299" s="4" t="inlineStr"/>
       <c r="H299" s="4" t="inlineStr"/>
       <c r="I299" s="4" t="inlineStr"/>
-      <c r="J299" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J299" s="6" t="n"/>
       <c r="K299" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L299" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M299" s="4" t="inlineStr">
@@ -21529,19 +21297,15 @@
       <c r="G302" s="4" t="inlineStr"/>
       <c r="H302" s="4" t="inlineStr"/>
       <c r="I302" s="4" t="inlineStr"/>
-      <c r="J302" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J302" s="6" t="n"/>
       <c r="K302" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L302" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M302" s="4" t="inlineStr">
@@ -21818,19 +21582,15 @@
       <c r="G306" s="4" t="inlineStr"/>
       <c r="H306" s="4" t="inlineStr"/>
       <c r="I306" s="4" t="inlineStr"/>
-      <c r="J306" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J306" s="6" t="n"/>
       <c r="K306" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L306" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M306" s="4" t="inlineStr">
@@ -22308,19 +22068,15 @@
       <c r="G313" s="4" t="inlineStr"/>
       <c r="H313" s="4" t="inlineStr"/>
       <c r="I313" s="4" t="inlineStr"/>
-      <c r="J313" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J313" s="6" t="n"/>
       <c r="K313" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L313" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M313" s="4" t="inlineStr">
@@ -22451,19 +22207,15 @@
       <c r="G315" s="4" t="inlineStr"/>
       <c r="H315" s="4" t="inlineStr"/>
       <c r="I315" s="4" t="inlineStr"/>
-      <c r="J315" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J315" s="6" t="n"/>
       <c r="K315" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L315" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M315" s="4" t="inlineStr">
@@ -22812,19 +22564,15 @@
       <c r="G320" s="4" t="inlineStr"/>
       <c r="H320" s="4" t="inlineStr"/>
       <c r="I320" s="4" t="inlineStr"/>
-      <c r="J320" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J320" s="6" t="n"/>
       <c r="K320" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L320" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M320" s="4" t="inlineStr">
@@ -22880,19 +22628,15 @@
       <c r="G321" s="4" t="inlineStr"/>
       <c r="H321" s="4" t="inlineStr"/>
       <c r="I321" s="4" t="inlineStr"/>
-      <c r="J321" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J321" s="6" t="n"/>
       <c r="K321" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L321" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M321" s="4" t="inlineStr">
@@ -22948,19 +22692,15 @@
       <c r="G322" s="4" t="inlineStr"/>
       <c r="H322" s="4" t="inlineStr"/>
       <c r="I322" s="4" t="inlineStr"/>
-      <c r="J322" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J322" s="6" t="n"/>
       <c r="K322" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L322" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M322" s="4" t="inlineStr">
@@ -23091,19 +22831,15 @@
       <c r="G324" s="4" t="inlineStr"/>
       <c r="H324" s="4" t="inlineStr"/>
       <c r="I324" s="4" t="inlineStr"/>
-      <c r="J324" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J324" s="6" t="n"/>
       <c r="K324" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L324" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M324" s="4" t="inlineStr">
@@ -23159,19 +22895,15 @@
       <c r="G325" s="4" t="inlineStr"/>
       <c r="H325" s="4" t="inlineStr"/>
       <c r="I325" s="4" t="inlineStr"/>
-      <c r="J325" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J325" s="6" t="n"/>
       <c r="K325" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L325" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M325" s="4" t="inlineStr">
@@ -24533,19 +24265,15 @@
       <c r="G344" s="4" t="inlineStr"/>
       <c r="H344" s="4" t="inlineStr"/>
       <c r="I344" s="4" t="inlineStr"/>
-      <c r="J344" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J344" s="6" t="n"/>
       <c r="K344" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L344" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M344" s="4" t="inlineStr">
@@ -24751,19 +24479,15 @@
       <c r="G347" s="4" t="inlineStr"/>
       <c r="H347" s="4" t="inlineStr"/>
       <c r="I347" s="4" t="inlineStr"/>
-      <c r="J347" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J347" s="6" t="n"/>
       <c r="K347" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L347" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M347" s="4" t="inlineStr">
@@ -24819,19 +24543,15 @@
       <c r="G348" s="4" t="inlineStr"/>
       <c r="H348" s="4" t="inlineStr"/>
       <c r="I348" s="4" t="inlineStr"/>
-      <c r="J348" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J348" s="6" t="n"/>
       <c r="K348" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L348" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M348" s="4" t="inlineStr">
@@ -24962,19 +24682,15 @@
       <c r="G350" s="4" t="inlineStr"/>
       <c r="H350" s="4" t="inlineStr"/>
       <c r="I350" s="4" t="inlineStr"/>
-      <c r="J350" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J350" s="6" t="n"/>
       <c r="K350" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L350" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M350" s="4" t="inlineStr">
@@ -25030,19 +24746,15 @@
       <c r="G351" s="4" t="inlineStr"/>
       <c r="H351" s="4" t="inlineStr"/>
       <c r="I351" s="4" t="inlineStr"/>
-      <c r="J351" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J351" s="6" t="n"/>
       <c r="K351" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L351" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M351" s="4" t="inlineStr">
@@ -25170,19 +24882,15 @@
       <c r="G353" s="4" t="inlineStr"/>
       <c r="H353" s="4" t="inlineStr"/>
       <c r="I353" s="4" t="inlineStr"/>
-      <c r="J353" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J353" s="6" t="n"/>
       <c r="K353" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L353" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M353" s="4" t="inlineStr">
@@ -25556,19 +25264,15 @@
       <c r="G359" s="4" t="inlineStr"/>
       <c r="H359" s="4" t="inlineStr"/>
       <c r="I359" s="4" t="inlineStr"/>
-      <c r="J359" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J359" s="6" t="n"/>
       <c r="K359" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L359" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M359" s="4" t="inlineStr">
@@ -26314,19 +26018,15 @@
       <c r="G370" s="4" t="inlineStr"/>
       <c r="H370" s="4" t="inlineStr"/>
       <c r="I370" s="4" t="inlineStr"/>
-      <c r="J370" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J370" s="6" t="n"/>
       <c r="K370" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L370" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M370" s="4" t="inlineStr">
@@ -27751,19 +27451,15 @@
       <c r="G391" s="4" t="inlineStr"/>
       <c r="H391" s="4" t="inlineStr"/>
       <c r="I391" s="4" t="inlineStr"/>
-      <c r="J391" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J391" s="6" t="n"/>
       <c r="K391" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L391" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M391" s="4" t="inlineStr">
@@ -27819,19 +27515,15 @@
       <c r="G392" s="4" t="inlineStr"/>
       <c r="H392" s="4" t="inlineStr"/>
       <c r="I392" s="4" t="inlineStr"/>
-      <c r="J392" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J392" s="6" t="n"/>
       <c r="K392" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L392" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M392" s="4" t="inlineStr">
@@ -28372,19 +28064,15 @@
       <c r="G400" s="4" t="inlineStr"/>
       <c r="H400" s="4" t="inlineStr"/>
       <c r="I400" s="4" t="inlineStr"/>
-      <c r="J400" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J400" s="6" t="n"/>
       <c r="K400" s="7" t="inlineStr">
         <is>
-          <t>AFTER_HIT</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L400" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M400" s="4" t="inlineStr">
@@ -28440,19 +28128,15 @@
       <c r="G401" s="4" t="inlineStr"/>
       <c r="H401" s="4" t="inlineStr"/>
       <c r="I401" s="4" t="inlineStr"/>
-      <c r="J401" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J401" s="6" t="n"/>
       <c r="K401" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L401" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M401" s="4" t="inlineStr">
@@ -28508,19 +28192,15 @@
       <c r="G402" s="4" t="inlineStr"/>
       <c r="H402" s="4" t="inlineStr"/>
       <c r="I402" s="4" t="inlineStr"/>
-      <c r="J402" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J402" s="6" t="n"/>
       <c r="K402" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L402" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M402" s="4" t="inlineStr">
@@ -28783,19 +28463,15 @@
       <c r="G406" s="4" t="inlineStr"/>
       <c r="H406" s="4" t="inlineStr"/>
       <c r="I406" s="4" t="inlineStr"/>
-      <c r="J406" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J406" s="6" t="n"/>
       <c r="K406" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L406" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M406" s="4" t="inlineStr">
@@ -28998,19 +28674,15 @@
       <c r="G409" s="4" t="inlineStr"/>
       <c r="H409" s="4" t="inlineStr"/>
       <c r="I409" s="4" t="inlineStr"/>
-      <c r="J409" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J409" s="6" t="n"/>
       <c r="K409" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L409" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M409" s="4" t="inlineStr">
@@ -29066,19 +28738,15 @@
       <c r="G410" s="4" t="inlineStr"/>
       <c r="H410" s="4" t="inlineStr"/>
       <c r="I410" s="4" t="inlineStr"/>
-      <c r="J410" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J410" s="6" t="n"/>
       <c r="K410" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L410" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M410" s="4" t="inlineStr">
@@ -29784,19 +29452,15 @@
       <c r="G420" s="4" t="inlineStr"/>
       <c r="H420" s="4" t="inlineStr"/>
       <c r="I420" s="4" t="inlineStr"/>
-      <c r="J420" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J420" s="6" t="n"/>
       <c r="K420" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L420" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M420" s="4" t="inlineStr">
@@ -30063,19 +29727,15 @@
       <c r="G424" s="4" t="inlineStr"/>
       <c r="H424" s="4" t="inlineStr"/>
       <c r="I424" s="4" t="inlineStr"/>
-      <c r="J424" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J424" s="6" t="n"/>
       <c r="K424" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L424" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M424" s="4" t="inlineStr">
@@ -30131,19 +29791,15 @@
       <c r="G425" s="4" t="inlineStr"/>
       <c r="H425" s="4" t="inlineStr"/>
       <c r="I425" s="4" t="inlineStr"/>
-      <c r="J425" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J425" s="6" t="n"/>
       <c r="K425" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L425" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M425" s="4" t="inlineStr">
@@ -30199,19 +29855,15 @@
       <c r="G426" s="4" t="inlineStr"/>
       <c r="H426" s="4" t="inlineStr"/>
       <c r="I426" s="4" t="inlineStr"/>
-      <c r="J426" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J426" s="6" t="n"/>
       <c r="K426" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L426" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M426" s="4" t="inlineStr">
@@ -30848,19 +30500,15 @@
       <c r="G436" s="4" t="inlineStr"/>
       <c r="H436" s="4" t="inlineStr"/>
       <c r="I436" s="4" t="inlineStr"/>
-      <c r="J436" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J436" s="6" t="n"/>
       <c r="K436" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L436" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M436" s="4" t="inlineStr">
@@ -31268,10 +30916,10 @@
         </is>
       </c>
       <c r="I442" s="4" t="inlineStr"/>
-      <c r="J442" s="4" t="inlineStr"/>
+      <c r="J442" s="4" t="n"/>
       <c r="K442" s="7" t="inlineStr">
         <is>
-          <t>DIRECT_DAMAGE</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L442" s="7" t="inlineStr">
@@ -31340,10 +30988,10 @@
         </is>
       </c>
       <c r="I443" s="4" t="inlineStr"/>
-      <c r="J443" s="4" t="inlineStr"/>
+      <c r="J443" s="4" t="n"/>
       <c r="K443" s="7" t="inlineStr">
         <is>
-          <t>DIRECT_DAMAGE</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L443" s="7" t="inlineStr">
@@ -31412,10 +31060,10 @@
         </is>
       </c>
       <c r="I444" s="4" t="inlineStr"/>
-      <c r="J444" s="4" t="inlineStr"/>
+      <c r="J444" s="4" t="n"/>
       <c r="K444" s="7" t="inlineStr">
         <is>
-          <t>DIRECT_DAMAGE</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L444" s="7" t="inlineStr">
@@ -31476,19 +31124,15 @@
       <c r="G445" s="4" t="inlineStr"/>
       <c r="H445" s="4" t="inlineStr"/>
       <c r="I445" s="4" t="inlineStr"/>
-      <c r="J445" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J445" s="6" t="n"/>
       <c r="K445" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L445" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M445" s="4" t="inlineStr">
@@ -31552,10 +31196,10 @@
         </is>
       </c>
       <c r="I446" s="4" t="inlineStr"/>
-      <c r="J446" s="4" t="inlineStr"/>
+      <c r="J446" s="4" t="n"/>
       <c r="K446" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L446" s="7" t="inlineStr">
@@ -31906,15 +31550,15 @@
       <c r="G451" s="4" t="inlineStr"/>
       <c r="H451" s="4" t="inlineStr"/>
       <c r="I451" s="4" t="inlineStr"/>
-      <c r="J451" s="4" t="inlineStr"/>
+      <c r="J451" s="4" t="n"/>
       <c r="K451" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L451" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M451" s="4" t="inlineStr">
@@ -32240,19 +31884,15 @@
       <c r="G456" s="4" t="inlineStr"/>
       <c r="H456" s="4" t="inlineStr"/>
       <c r="I456" s="4" t="inlineStr"/>
-      <c r="J456" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J456" s="6" t="n"/>
       <c r="K456" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L456" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M456" s="4" t="inlineStr">
@@ -33115,19 +32755,15 @@
       <c r="G469" s="4" t="inlineStr"/>
       <c r="H469" s="4" t="inlineStr"/>
       <c r="I469" s="4" t="inlineStr"/>
-      <c r="J469" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J469" s="6" t="n"/>
       <c r="K469" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L469" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M469" s="4" t="inlineStr">
@@ -33183,19 +32819,15 @@
       <c r="G470" s="4" t="inlineStr"/>
       <c r="H470" s="4" t="inlineStr"/>
       <c r="I470" s="4" t="inlineStr"/>
-      <c r="J470" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J470" s="6" t="n"/>
       <c r="K470" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L470" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M470" s="4" t="inlineStr">
@@ -34450,19 +34082,15 @@
       <c r="G488" s="4" t="inlineStr"/>
       <c r="H488" s="4" t="inlineStr"/>
       <c r="I488" s="4" t="inlineStr"/>
-      <c r="J488" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J488" s="6" t="n"/>
       <c r="K488" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L488" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M488" s="4" t="inlineStr">
@@ -34937,19 +34565,15 @@
       <c r="G495" s="4" t="inlineStr"/>
       <c r="H495" s="4" t="inlineStr"/>
       <c r="I495" s="4" t="inlineStr"/>
-      <c r="J495" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J495" s="6" t="n"/>
       <c r="K495" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L495" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M495" s="4" t="inlineStr">
@@ -35005,19 +34629,15 @@
       <c r="G496" s="4" t="inlineStr"/>
       <c r="H496" s="4" t="inlineStr"/>
       <c r="I496" s="4" t="inlineStr"/>
-      <c r="J496" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J496" s="6" t="n"/>
       <c r="K496" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L496" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M496" s="4" t="inlineStr">
@@ -35141,19 +34761,15 @@
       <c r="G498" s="4" t="inlineStr"/>
       <c r="H498" s="4" t="inlineStr"/>
       <c r="I498" s="4" t="inlineStr"/>
-      <c r="J498" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J498" s="6" t="n"/>
       <c r="K498" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L498" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M498" s="4" t="inlineStr">
@@ -35419,19 +35035,15 @@
       <c r="G502" s="4" t="inlineStr"/>
       <c r="H502" s="4" t="inlineStr"/>
       <c r="I502" s="4" t="inlineStr"/>
-      <c r="J502" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J502" s="6" t="n"/>
       <c r="K502" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L502" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M502" s="4" t="inlineStr">
@@ -35487,19 +35099,15 @@
       <c r="G503" s="4" t="inlineStr"/>
       <c r="H503" s="4" t="inlineStr"/>
       <c r="I503" s="4" t="inlineStr"/>
-      <c r="J503" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J503" s="6" t="n"/>
       <c r="K503" s="7" t="inlineStr">
         <is>
-          <t>PRE_ATTACK</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L503" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M503" s="4" t="inlineStr">
@@ -35683,19 +35291,15 @@
       <c r="G506" s="4" t="inlineStr"/>
       <c r="H506" s="4" t="inlineStr"/>
       <c r="I506" s="4" t="inlineStr"/>
-      <c r="J506" s="6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
+      <c r="J506" s="6" t="n"/>
       <c r="K506" s="7" t="inlineStr">
         <is>
-          <t>CALC_AP</t>
+          <t>ACTIVATION_START</t>
         </is>
       </c>
       <c r="L506" s="7" t="inlineStr">
         <is>
-          <t>always</t>
+          <t>once_per_activation</t>
         </is>
       </c>
       <c r="M506" s="4" t="inlineStr">

</xml_diff>